<commit_message>
Change Flag country to Flag state
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1DI.xlsx
+++ b/form_reporting_templates/Form-1DI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C86E388-0B27-4727-8A30-C0AC001530BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7C7E6-32F4-4A4D-A566-5AB77EA5C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>General information</t>
-  </si>
-  <si>
-    <t>Flag country</t>
   </si>
   <si>
     <t>Reporting year</t>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>IOTC Form 1DI | data</t>
+  </si>
+  <si>
+    <t>Flag state</t>
   </si>
 </sst>
 </file>
@@ -933,9 +933,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1140,6 +1137,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1489,39 +1489,39 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
-        <v>33</v>
+      <c r="B2" s="83" t="s">
+        <v>32</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="86"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="87"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="88"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1537,7 +1537,7 @@
     <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="9"/>
       <c r="C6" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1556,15 +1556,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="83" t="s">
-        <v>28</v>
+      <c r="F8" s="82" t="s">
+        <v>27</v>
       </c>
-      <c r="G8" s="83"/>
+      <c r="G8" s="82"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1583,12 +1583,12 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="11"/>
@@ -1605,7 +1605,7 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="10"/>
@@ -1616,7 +1616,7 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="10"/>
@@ -1665,7 +1665,7 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="40"/>
       <c r="E18" s="10"/>
@@ -1675,8 +1675,8 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="53" t="s">
-        <v>24</v>
+      <c r="C19" s="52" t="s">
+        <v>23</v>
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="10"/>
@@ -1686,8 +1686,8 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="52" t="s">
-        <v>4</v>
+      <c r="C20" s="112" t="s">
+        <v>34</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="10"/>
@@ -1716,7 +1716,7 @@
     <row r="23" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="10"/>
@@ -1735,11 +1735,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="82"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="81"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1756,21 +1756,24 @@
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="s5sWwGU39K/jsjWkGeSh8ojbl3IMfuYvo2yvQ9PDCGhkZMOyxmWVphJ9NV9JxN1SK+HZaDh7ZhWMcjBzxaxoOA==" saltValue="t9NLa2hLggW8kdm4G9FjFQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2UXIQAtCAe1Hl3LOIP95j6T5lN4CreFbp/G7xZfYEjLnpx98jtQhpQhWmp07FYOVM1xMp78hncUia1FB6wrMWw==" saltValue="HvcaMeX3WSxt5je20kTU3g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B2:H3"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C20" xr:uid="{B9CB61C8-BBA2-4A24-8E84-84C263F59204}">
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{B9CB61C8-BBA2-4A24-8E84-84C263F59204}">
+      <formula1>"&lt;0&gt;0"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20" xr:uid="{84E8478B-349E-439F-A70D-E4E827D455F5}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C19" r:id="rId1" location="entities" xr:uid="{3E135360-8976-4AAA-8474-BB32F06C9745}"/>
-    <hyperlink ref="C20" r:id="rId2" location="countries" xr:uid="{F730E8AF-D3A7-4431-9DD3-422CC542A285}"/>
+    <hyperlink ref="C20" r:id="rId2" location="countries" display="Flag country" xr:uid="{F730E8AF-D3A7-4431-9DD3-422CC542A285}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1791,19 +1794,19 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="65" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="66" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="66" customWidth="1"/>
-    <col min="5" max="5" width="14" style="67" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="65" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="66" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="68" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="65" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="71" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="79" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="75"/>
-    <col min="13" max="210" width="9.140625" style="76"/>
-    <col min="211" max="211" width="9.140625" style="77"/>
+    <col min="2" max="2" width="11.42578125" style="64" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="65" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="65" customWidth="1"/>
+    <col min="5" max="5" width="14" style="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="64" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="65" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="67" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="64" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="70" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="74"/>
+    <col min="13" max="210" width="9.140625" style="75"/>
+    <col min="211" max="211" width="9.140625" style="76"/>
     <col min="212" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
@@ -1811,18 +1814,18 @@
       <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="84" t="s">
-        <v>34</v>
+      <c r="B2" s="83" t="s">
+        <v>33</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="111"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
@@ -2026,237 +2029,237 @@
     </row>
     <row r="3" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="108" t="s">
-        <v>27</v>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="107" t="s">
+        <v>26</v>
       </c>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="109"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="109"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="109"/>
-      <c r="AA3" s="109"/>
-      <c r="AB3" s="109"/>
-      <c r="AC3" s="109"/>
-      <c r="AD3" s="109"/>
-      <c r="AE3" s="109"/>
-      <c r="AF3" s="109"/>
-      <c r="AG3" s="109"/>
-      <c r="AH3" s="109"/>
-      <c r="AI3" s="109"/>
-      <c r="AJ3" s="109"/>
-      <c r="AK3" s="109"/>
-      <c r="AL3" s="109"/>
-      <c r="AM3" s="109"/>
-      <c r="AN3" s="109"/>
-      <c r="AO3" s="109"/>
-      <c r="AP3" s="109"/>
-      <c r="AQ3" s="109"/>
-      <c r="AR3" s="109"/>
-      <c r="AS3" s="109"/>
-      <c r="AT3" s="109"/>
-      <c r="AU3" s="109"/>
-      <c r="AV3" s="109"/>
-      <c r="AW3" s="109"/>
-      <c r="AX3" s="109"/>
-      <c r="AY3" s="109"/>
-      <c r="AZ3" s="109"/>
-      <c r="BA3" s="109"/>
-      <c r="BB3" s="109"/>
-      <c r="BC3" s="109"/>
-      <c r="BD3" s="109"/>
-      <c r="BE3" s="109"/>
-      <c r="BF3" s="109"/>
-      <c r="BG3" s="109"/>
-      <c r="BH3" s="109"/>
-      <c r="BI3" s="109"/>
-      <c r="BJ3" s="109"/>
-      <c r="BK3" s="109"/>
-      <c r="BL3" s="109"/>
-      <c r="BM3" s="109"/>
-      <c r="BN3" s="109"/>
-      <c r="BO3" s="109"/>
-      <c r="BP3" s="109"/>
-      <c r="BQ3" s="109"/>
-      <c r="BR3" s="109"/>
-      <c r="BS3" s="109"/>
-      <c r="BT3" s="109"/>
-      <c r="BU3" s="109"/>
-      <c r="BV3" s="109"/>
-      <c r="BW3" s="109"/>
-      <c r="BX3" s="109"/>
-      <c r="BY3" s="109"/>
-      <c r="BZ3" s="109"/>
-      <c r="CA3" s="109"/>
-      <c r="CB3" s="109"/>
-      <c r="CC3" s="109"/>
-      <c r="CD3" s="109"/>
-      <c r="CE3" s="109"/>
-      <c r="CF3" s="109"/>
-      <c r="CG3" s="109"/>
-      <c r="CH3" s="109"/>
-      <c r="CI3" s="109"/>
-      <c r="CJ3" s="109"/>
-      <c r="CK3" s="109"/>
-      <c r="CL3" s="109"/>
-      <c r="CM3" s="109"/>
-      <c r="CN3" s="109"/>
-      <c r="CO3" s="109"/>
-      <c r="CP3" s="109"/>
-      <c r="CQ3" s="109"/>
-      <c r="CR3" s="109"/>
-      <c r="CS3" s="109"/>
-      <c r="CT3" s="109"/>
-      <c r="CU3" s="109"/>
-      <c r="CV3" s="109"/>
-      <c r="CW3" s="109"/>
-      <c r="CX3" s="109"/>
-      <c r="CY3" s="109"/>
-      <c r="CZ3" s="109"/>
-      <c r="DA3" s="109"/>
-      <c r="DB3" s="109"/>
-      <c r="DC3" s="109"/>
-      <c r="DD3" s="109"/>
-      <c r="DE3" s="109"/>
-      <c r="DF3" s="109"/>
-      <c r="DG3" s="109"/>
-      <c r="DH3" s="109"/>
-      <c r="DI3" s="109"/>
-      <c r="DJ3" s="109"/>
-      <c r="DK3" s="109"/>
-      <c r="DL3" s="109"/>
-      <c r="DM3" s="109"/>
-      <c r="DN3" s="109"/>
-      <c r="DO3" s="109"/>
-      <c r="DP3" s="109"/>
-      <c r="DQ3" s="109"/>
-      <c r="DR3" s="109"/>
-      <c r="DS3" s="109"/>
-      <c r="DT3" s="109"/>
-      <c r="DU3" s="109"/>
-      <c r="DV3" s="109"/>
-      <c r="DW3" s="109"/>
-      <c r="DX3" s="109"/>
-      <c r="DY3" s="109"/>
-      <c r="DZ3" s="109"/>
-      <c r="EA3" s="109"/>
-      <c r="EB3" s="109"/>
-      <c r="EC3" s="109"/>
-      <c r="ED3" s="109"/>
-      <c r="EE3" s="109"/>
-      <c r="EF3" s="109"/>
-      <c r="EG3" s="109"/>
-      <c r="EH3" s="109"/>
-      <c r="EI3" s="109"/>
-      <c r="EJ3" s="109"/>
-      <c r="EK3" s="109"/>
-      <c r="EL3" s="109"/>
-      <c r="EM3" s="109"/>
-      <c r="EN3" s="109"/>
-      <c r="EO3" s="109"/>
-      <c r="EP3" s="109"/>
-      <c r="EQ3" s="109"/>
-      <c r="ER3" s="109"/>
-      <c r="ES3" s="109"/>
-      <c r="ET3" s="109"/>
-      <c r="EU3" s="109"/>
-      <c r="EV3" s="109"/>
-      <c r="EW3" s="109"/>
-      <c r="EX3" s="109"/>
-      <c r="EY3" s="109"/>
-      <c r="EZ3" s="109"/>
-      <c r="FA3" s="109"/>
-      <c r="FB3" s="109"/>
-      <c r="FC3" s="109"/>
-      <c r="FD3" s="109"/>
-      <c r="FE3" s="109"/>
-      <c r="FF3" s="109"/>
-      <c r="FG3" s="109"/>
-      <c r="FH3" s="109"/>
-      <c r="FI3" s="109"/>
-      <c r="FJ3" s="109"/>
-      <c r="FK3" s="109"/>
-      <c r="FL3" s="109"/>
-      <c r="FM3" s="109"/>
-      <c r="FN3" s="109"/>
-      <c r="FO3" s="109"/>
-      <c r="FP3" s="109"/>
-      <c r="FQ3" s="109"/>
-      <c r="FR3" s="109"/>
-      <c r="FS3" s="109"/>
-      <c r="FT3" s="109"/>
-      <c r="FU3" s="109"/>
-      <c r="FV3" s="109"/>
-      <c r="FW3" s="109"/>
-      <c r="FX3" s="109"/>
-      <c r="FY3" s="109"/>
-      <c r="FZ3" s="109"/>
-      <c r="GA3" s="109"/>
-      <c r="GB3" s="109"/>
-      <c r="GC3" s="109"/>
-      <c r="GD3" s="109"/>
-      <c r="GE3" s="109"/>
-      <c r="GF3" s="109"/>
-      <c r="GG3" s="109"/>
-      <c r="GH3" s="109"/>
-      <c r="GI3" s="109"/>
-      <c r="GJ3" s="109"/>
-      <c r="GK3" s="109"/>
-      <c r="GL3" s="109"/>
-      <c r="GM3" s="109"/>
-      <c r="GN3" s="109"/>
-      <c r="GO3" s="109"/>
-      <c r="GP3" s="109"/>
-      <c r="GQ3" s="109"/>
-      <c r="GR3" s="109"/>
-      <c r="GS3" s="109"/>
-      <c r="GT3" s="109"/>
-      <c r="GU3" s="109"/>
-      <c r="GV3" s="109"/>
-      <c r="GW3" s="109"/>
-      <c r="GX3" s="109"/>
-      <c r="GY3" s="109"/>
-      <c r="GZ3" s="109"/>
-      <c r="HA3" s="109"/>
-      <c r="HB3" s="109"/>
-      <c r="HC3" s="110"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="108"/>
+      <c r="Y3" s="108"/>
+      <c r="Z3" s="108"/>
+      <c r="AA3" s="108"/>
+      <c r="AB3" s="108"/>
+      <c r="AC3" s="108"/>
+      <c r="AD3" s="108"/>
+      <c r="AE3" s="108"/>
+      <c r="AF3" s="108"/>
+      <c r="AG3" s="108"/>
+      <c r="AH3" s="108"/>
+      <c r="AI3" s="108"/>
+      <c r="AJ3" s="108"/>
+      <c r="AK3" s="108"/>
+      <c r="AL3" s="108"/>
+      <c r="AM3" s="108"/>
+      <c r="AN3" s="108"/>
+      <c r="AO3" s="108"/>
+      <c r="AP3" s="108"/>
+      <c r="AQ3" s="108"/>
+      <c r="AR3" s="108"/>
+      <c r="AS3" s="108"/>
+      <c r="AT3" s="108"/>
+      <c r="AU3" s="108"/>
+      <c r="AV3" s="108"/>
+      <c r="AW3" s="108"/>
+      <c r="AX3" s="108"/>
+      <c r="AY3" s="108"/>
+      <c r="AZ3" s="108"/>
+      <c r="BA3" s="108"/>
+      <c r="BB3" s="108"/>
+      <c r="BC3" s="108"/>
+      <c r="BD3" s="108"/>
+      <c r="BE3" s="108"/>
+      <c r="BF3" s="108"/>
+      <c r="BG3" s="108"/>
+      <c r="BH3" s="108"/>
+      <c r="BI3" s="108"/>
+      <c r="BJ3" s="108"/>
+      <c r="BK3" s="108"/>
+      <c r="BL3" s="108"/>
+      <c r="BM3" s="108"/>
+      <c r="BN3" s="108"/>
+      <c r="BO3" s="108"/>
+      <c r="BP3" s="108"/>
+      <c r="BQ3" s="108"/>
+      <c r="BR3" s="108"/>
+      <c r="BS3" s="108"/>
+      <c r="BT3" s="108"/>
+      <c r="BU3" s="108"/>
+      <c r="BV3" s="108"/>
+      <c r="BW3" s="108"/>
+      <c r="BX3" s="108"/>
+      <c r="BY3" s="108"/>
+      <c r="BZ3" s="108"/>
+      <c r="CA3" s="108"/>
+      <c r="CB3" s="108"/>
+      <c r="CC3" s="108"/>
+      <c r="CD3" s="108"/>
+      <c r="CE3" s="108"/>
+      <c r="CF3" s="108"/>
+      <c r="CG3" s="108"/>
+      <c r="CH3" s="108"/>
+      <c r="CI3" s="108"/>
+      <c r="CJ3" s="108"/>
+      <c r="CK3" s="108"/>
+      <c r="CL3" s="108"/>
+      <c r="CM3" s="108"/>
+      <c r="CN3" s="108"/>
+      <c r="CO3" s="108"/>
+      <c r="CP3" s="108"/>
+      <c r="CQ3" s="108"/>
+      <c r="CR3" s="108"/>
+      <c r="CS3" s="108"/>
+      <c r="CT3" s="108"/>
+      <c r="CU3" s="108"/>
+      <c r="CV3" s="108"/>
+      <c r="CW3" s="108"/>
+      <c r="CX3" s="108"/>
+      <c r="CY3" s="108"/>
+      <c r="CZ3" s="108"/>
+      <c r="DA3" s="108"/>
+      <c r="DB3" s="108"/>
+      <c r="DC3" s="108"/>
+      <c r="DD3" s="108"/>
+      <c r="DE3" s="108"/>
+      <c r="DF3" s="108"/>
+      <c r="DG3" s="108"/>
+      <c r="DH3" s="108"/>
+      <c r="DI3" s="108"/>
+      <c r="DJ3" s="108"/>
+      <c r="DK3" s="108"/>
+      <c r="DL3" s="108"/>
+      <c r="DM3" s="108"/>
+      <c r="DN3" s="108"/>
+      <c r="DO3" s="108"/>
+      <c r="DP3" s="108"/>
+      <c r="DQ3" s="108"/>
+      <c r="DR3" s="108"/>
+      <c r="DS3" s="108"/>
+      <c r="DT3" s="108"/>
+      <c r="DU3" s="108"/>
+      <c r="DV3" s="108"/>
+      <c r="DW3" s="108"/>
+      <c r="DX3" s="108"/>
+      <c r="DY3" s="108"/>
+      <c r="DZ3" s="108"/>
+      <c r="EA3" s="108"/>
+      <c r="EB3" s="108"/>
+      <c r="EC3" s="108"/>
+      <c r="ED3" s="108"/>
+      <c r="EE3" s="108"/>
+      <c r="EF3" s="108"/>
+      <c r="EG3" s="108"/>
+      <c r="EH3" s="108"/>
+      <c r="EI3" s="108"/>
+      <c r="EJ3" s="108"/>
+      <c r="EK3" s="108"/>
+      <c r="EL3" s="108"/>
+      <c r="EM3" s="108"/>
+      <c r="EN3" s="108"/>
+      <c r="EO3" s="108"/>
+      <c r="EP3" s="108"/>
+      <c r="EQ3" s="108"/>
+      <c r="ER3" s="108"/>
+      <c r="ES3" s="108"/>
+      <c r="ET3" s="108"/>
+      <c r="EU3" s="108"/>
+      <c r="EV3" s="108"/>
+      <c r="EW3" s="108"/>
+      <c r="EX3" s="108"/>
+      <c r="EY3" s="108"/>
+      <c r="EZ3" s="108"/>
+      <c r="FA3" s="108"/>
+      <c r="FB3" s="108"/>
+      <c r="FC3" s="108"/>
+      <c r="FD3" s="108"/>
+      <c r="FE3" s="108"/>
+      <c r="FF3" s="108"/>
+      <c r="FG3" s="108"/>
+      <c r="FH3" s="108"/>
+      <c r="FI3" s="108"/>
+      <c r="FJ3" s="108"/>
+      <c r="FK3" s="108"/>
+      <c r="FL3" s="108"/>
+      <c r="FM3" s="108"/>
+      <c r="FN3" s="108"/>
+      <c r="FO3" s="108"/>
+      <c r="FP3" s="108"/>
+      <c r="FQ3" s="108"/>
+      <c r="FR3" s="108"/>
+      <c r="FS3" s="108"/>
+      <c r="FT3" s="108"/>
+      <c r="FU3" s="108"/>
+      <c r="FV3" s="108"/>
+      <c r="FW3" s="108"/>
+      <c r="FX3" s="108"/>
+      <c r="FY3" s="108"/>
+      <c r="FZ3" s="108"/>
+      <c r="GA3" s="108"/>
+      <c r="GB3" s="108"/>
+      <c r="GC3" s="108"/>
+      <c r="GD3" s="108"/>
+      <c r="GE3" s="108"/>
+      <c r="GF3" s="108"/>
+      <c r="GG3" s="108"/>
+      <c r="GH3" s="108"/>
+      <c r="GI3" s="108"/>
+      <c r="GJ3" s="108"/>
+      <c r="GK3" s="108"/>
+      <c r="GL3" s="108"/>
+      <c r="GM3" s="108"/>
+      <c r="GN3" s="108"/>
+      <c r="GO3" s="108"/>
+      <c r="GP3" s="108"/>
+      <c r="GQ3" s="108"/>
+      <c r="GR3" s="108"/>
+      <c r="GS3" s="108"/>
+      <c r="GT3" s="108"/>
+      <c r="GU3" s="108"/>
+      <c r="GV3" s="108"/>
+      <c r="GW3" s="108"/>
+      <c r="GX3" s="108"/>
+      <c r="GY3" s="108"/>
+      <c r="GZ3" s="108"/>
+      <c r="HA3" s="108"/>
+      <c r="HB3" s="108"/>
+      <c r="HC3" s="109"/>
     </row>
     <row r="4" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="90" t="s">
-        <v>22</v>
+      <c r="B4" s="89" t="s">
+        <v>21</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="99" t="s">
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="98" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="100"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="99" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="101"/>
-      <c r="K4" s="63" t="s">
-        <v>13</v>
+      <c r="J4" s="100"/>
+      <c r="K4" s="62" t="s">
+        <v>12</v>
       </c>
       <c r="L4" s="26"/>
       <c r="M4" s="27"/>
@@ -2460,17 +2463,17 @@
       <c r="HC4" s="28"/>
     </row>
     <row r="5" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="93"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="104"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="103"/>
       <c r="K5" s="51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L5" s="26"/>
       <c r="M5" s="27"/>
@@ -2674,17 +2677,17 @@
       <c r="HC5" s="28"/>
     </row>
     <row r="6" spans="1:211" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="96"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="107"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="106"/>
       <c r="K6" s="51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L6" s="26"/>
       <c r="M6" s="27"/>
@@ -2888,35 +2891,35 @@
       <c r="HC6" s="28"/>
     </row>
     <row r="7" spans="1:211" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="54" t="s">
-        <v>11</v>
+      <c r="B7" s="53" t="s">
+        <v>10</v>
       </c>
-      <c r="C7" s="55" t="s">
-        <v>6</v>
+      <c r="C7" s="54" t="s">
+        <v>5</v>
       </c>
-      <c r="D7" s="56" t="s">
-        <v>23</v>
+      <c r="D7" s="55" t="s">
+        <v>22</v>
       </c>
-      <c r="E7" s="57" t="s">
-        <v>25</v>
+      <c r="E7" s="56" t="s">
+        <v>24</v>
       </c>
-      <c r="F7" s="60" t="s">
+      <c r="F7" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="58" t="s">
-        <v>17</v>
+      <c r="I7" s="60" t="s">
+        <v>14</v>
       </c>
-      <c r="H7" s="59" t="s">
-        <v>16</v>
+      <c r="J7" s="61" t="s">
+        <v>20</v>
       </c>
-      <c r="I7" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="64" t="s">
-        <v>26</v>
+      <c r="K7" s="63" t="s">
+        <v>25</v>
       </c>
       <c r="L7" s="29"/>
       <c r="M7" s="30"/>
@@ -3128,208 +3131,208 @@
       <c r="G8" s="43"/>
       <c r="H8" s="44"/>
       <c r="I8" s="45"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="73"/>
-      <c r="N8" s="73"/>
-      <c r="O8" s="73"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="73"/>
-      <c r="R8" s="73"/>
-      <c r="S8" s="73"/>
-      <c r="T8" s="73"/>
-      <c r="U8" s="73"/>
-      <c r="V8" s="73"/>
-      <c r="W8" s="73"/>
-      <c r="X8" s="73"/>
-      <c r="Y8" s="73"/>
-      <c r="Z8" s="73"/>
-      <c r="AA8" s="73"/>
-      <c r="AB8" s="73"/>
-      <c r="AC8" s="73"/>
-      <c r="AD8" s="73"/>
-      <c r="AE8" s="73"/>
-      <c r="AF8" s="73"/>
-      <c r="AG8" s="73"/>
-      <c r="AH8" s="73"/>
-      <c r="AI8" s="73"/>
-      <c r="AJ8" s="73"/>
-      <c r="AK8" s="73"/>
-      <c r="AL8" s="73"/>
-      <c r="AM8" s="73"/>
-      <c r="AN8" s="73"/>
-      <c r="AO8" s="73"/>
-      <c r="AP8" s="73"/>
-      <c r="AQ8" s="73"/>
-      <c r="AR8" s="73"/>
-      <c r="AS8" s="73"/>
-      <c r="AT8" s="73"/>
-      <c r="AU8" s="73"/>
-      <c r="AV8" s="73"/>
-      <c r="AW8" s="73"/>
-      <c r="AX8" s="73"/>
-      <c r="AY8" s="73"/>
-      <c r="AZ8" s="73"/>
-      <c r="BA8" s="73"/>
-      <c r="BB8" s="73"/>
-      <c r="BC8" s="73"/>
-      <c r="BD8" s="73"/>
-      <c r="BE8" s="73"/>
-      <c r="BF8" s="73"/>
-      <c r="BG8" s="73"/>
-      <c r="BH8" s="73"/>
-      <c r="BI8" s="73"/>
-      <c r="BJ8" s="73"/>
-      <c r="BK8" s="73"/>
-      <c r="BL8" s="73"/>
-      <c r="BM8" s="73"/>
-      <c r="BN8" s="73"/>
-      <c r="BO8" s="73"/>
-      <c r="BP8" s="73"/>
-      <c r="BQ8" s="73"/>
-      <c r="BR8" s="73"/>
-      <c r="BS8" s="73"/>
-      <c r="BT8" s="73"/>
-      <c r="BU8" s="73"/>
-      <c r="BV8" s="73"/>
-      <c r="BW8" s="73"/>
-      <c r="BX8" s="73"/>
-      <c r="BY8" s="73"/>
-      <c r="BZ8" s="73"/>
-      <c r="CA8" s="73"/>
-      <c r="CB8" s="73"/>
-      <c r="CC8" s="73"/>
-      <c r="CD8" s="73"/>
-      <c r="CE8" s="73"/>
-      <c r="CF8" s="73"/>
-      <c r="CG8" s="73"/>
-      <c r="CH8" s="73"/>
-      <c r="CI8" s="73"/>
-      <c r="CJ8" s="73"/>
-      <c r="CK8" s="73"/>
-      <c r="CL8" s="73"/>
-      <c r="CM8" s="73"/>
-      <c r="CN8" s="73"/>
-      <c r="CO8" s="73"/>
-      <c r="CP8" s="73"/>
-      <c r="CQ8" s="73"/>
-      <c r="CR8" s="73"/>
-      <c r="CS8" s="73"/>
-      <c r="CT8" s="73"/>
-      <c r="CU8" s="73"/>
-      <c r="CV8" s="73"/>
-      <c r="CW8" s="73"/>
-      <c r="CX8" s="73"/>
-      <c r="CY8" s="73"/>
-      <c r="CZ8" s="73"/>
-      <c r="DA8" s="73"/>
-      <c r="DB8" s="73"/>
-      <c r="DC8" s="73"/>
-      <c r="DD8" s="73"/>
-      <c r="DE8" s="73"/>
-      <c r="DF8" s="73"/>
-      <c r="DG8" s="73"/>
-      <c r="DH8" s="73"/>
-      <c r="DI8" s="73"/>
-      <c r="DJ8" s="73"/>
-      <c r="DK8" s="73"/>
-      <c r="DL8" s="73"/>
-      <c r="DM8" s="73"/>
-      <c r="DN8" s="73"/>
-      <c r="DO8" s="73"/>
-      <c r="DP8" s="73"/>
-      <c r="DQ8" s="73"/>
-      <c r="DR8" s="73"/>
-      <c r="DS8" s="73"/>
-      <c r="DT8" s="73"/>
-      <c r="DU8" s="73"/>
-      <c r="DV8" s="73"/>
-      <c r="DW8" s="73"/>
-      <c r="DX8" s="73"/>
-      <c r="DY8" s="73"/>
-      <c r="DZ8" s="73"/>
-      <c r="EA8" s="73"/>
-      <c r="EB8" s="73"/>
-      <c r="EC8" s="73"/>
-      <c r="ED8" s="73"/>
-      <c r="EE8" s="73"/>
-      <c r="EF8" s="73"/>
-      <c r="EG8" s="73"/>
-      <c r="EH8" s="73"/>
-      <c r="EI8" s="73"/>
-      <c r="EJ8" s="73"/>
-      <c r="EK8" s="73"/>
-      <c r="EL8" s="73"/>
-      <c r="EM8" s="73"/>
-      <c r="EN8" s="73"/>
-      <c r="EO8" s="73"/>
-      <c r="EP8" s="73"/>
-      <c r="EQ8" s="73"/>
-      <c r="ER8" s="73"/>
-      <c r="ES8" s="73"/>
-      <c r="ET8" s="73"/>
-      <c r="EU8" s="73"/>
-      <c r="EV8" s="73"/>
-      <c r="EW8" s="73"/>
-      <c r="EX8" s="73"/>
-      <c r="EY8" s="73"/>
-      <c r="EZ8" s="73"/>
-      <c r="FA8" s="73"/>
-      <c r="FB8" s="73"/>
-      <c r="FC8" s="73"/>
-      <c r="FD8" s="73"/>
-      <c r="FE8" s="73"/>
-      <c r="FF8" s="73"/>
-      <c r="FG8" s="73"/>
-      <c r="FH8" s="73"/>
-      <c r="FI8" s="73"/>
-      <c r="FJ8" s="73"/>
-      <c r="FK8" s="73"/>
-      <c r="FL8" s="73"/>
-      <c r="FM8" s="73"/>
-      <c r="FN8" s="73"/>
-      <c r="FO8" s="73"/>
-      <c r="FP8" s="73"/>
-      <c r="FQ8" s="73"/>
-      <c r="FR8" s="73"/>
-      <c r="FS8" s="73"/>
-      <c r="FT8" s="73"/>
-      <c r="FU8" s="73"/>
-      <c r="FV8" s="73"/>
-      <c r="FW8" s="73"/>
-      <c r="FX8" s="73"/>
-      <c r="FY8" s="73"/>
-      <c r="FZ8" s="73"/>
-      <c r="GA8" s="73"/>
-      <c r="GB8" s="73"/>
-      <c r="GC8" s="73"/>
-      <c r="GD8" s="73"/>
-      <c r="GE8" s="73"/>
-      <c r="GF8" s="73"/>
-      <c r="GG8" s="73"/>
-      <c r="GH8" s="73"/>
-      <c r="GI8" s="73"/>
-      <c r="GJ8" s="73"/>
-      <c r="GK8" s="73"/>
-      <c r="GL8" s="73"/>
-      <c r="GM8" s="73"/>
-      <c r="GN8" s="73"/>
-      <c r="GO8" s="73"/>
-      <c r="GP8" s="73"/>
-      <c r="GQ8" s="73"/>
-      <c r="GR8" s="73"/>
-      <c r="GS8" s="73"/>
-      <c r="GT8" s="73"/>
-      <c r="GU8" s="73"/>
-      <c r="GV8" s="73"/>
-      <c r="GW8" s="73"/>
-      <c r="GX8" s="73"/>
-      <c r="GY8" s="73"/>
-      <c r="GZ8" s="73"/>
-      <c r="HA8" s="73"/>
-      <c r="HB8" s="73"/>
-      <c r="HC8" s="74"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="72"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="72"/>
+      <c r="R8" s="72"/>
+      <c r="S8" s="72"/>
+      <c r="T8" s="72"/>
+      <c r="U8" s="72"/>
+      <c r="V8" s="72"/>
+      <c r="W8" s="72"/>
+      <c r="X8" s="72"/>
+      <c r="Y8" s="72"/>
+      <c r="Z8" s="72"/>
+      <c r="AA8" s="72"/>
+      <c r="AB8" s="72"/>
+      <c r="AC8" s="72"/>
+      <c r="AD8" s="72"/>
+      <c r="AE8" s="72"/>
+      <c r="AF8" s="72"/>
+      <c r="AG8" s="72"/>
+      <c r="AH8" s="72"/>
+      <c r="AI8" s="72"/>
+      <c r="AJ8" s="72"/>
+      <c r="AK8" s="72"/>
+      <c r="AL8" s="72"/>
+      <c r="AM8" s="72"/>
+      <c r="AN8" s="72"/>
+      <c r="AO8" s="72"/>
+      <c r="AP8" s="72"/>
+      <c r="AQ8" s="72"/>
+      <c r="AR8" s="72"/>
+      <c r="AS8" s="72"/>
+      <c r="AT8" s="72"/>
+      <c r="AU8" s="72"/>
+      <c r="AV8" s="72"/>
+      <c r="AW8" s="72"/>
+      <c r="AX8" s="72"/>
+      <c r="AY8" s="72"/>
+      <c r="AZ8" s="72"/>
+      <c r="BA8" s="72"/>
+      <c r="BB8" s="72"/>
+      <c r="BC8" s="72"/>
+      <c r="BD8" s="72"/>
+      <c r="BE8" s="72"/>
+      <c r="BF8" s="72"/>
+      <c r="BG8" s="72"/>
+      <c r="BH8" s="72"/>
+      <c r="BI8" s="72"/>
+      <c r="BJ8" s="72"/>
+      <c r="BK8" s="72"/>
+      <c r="BL8" s="72"/>
+      <c r="BM8" s="72"/>
+      <c r="BN8" s="72"/>
+      <c r="BO8" s="72"/>
+      <c r="BP8" s="72"/>
+      <c r="BQ8" s="72"/>
+      <c r="BR8" s="72"/>
+      <c r="BS8" s="72"/>
+      <c r="BT8" s="72"/>
+      <c r="BU8" s="72"/>
+      <c r="BV8" s="72"/>
+      <c r="BW8" s="72"/>
+      <c r="BX8" s="72"/>
+      <c r="BY8" s="72"/>
+      <c r="BZ8" s="72"/>
+      <c r="CA8" s="72"/>
+      <c r="CB8" s="72"/>
+      <c r="CC8" s="72"/>
+      <c r="CD8" s="72"/>
+      <c r="CE8" s="72"/>
+      <c r="CF8" s="72"/>
+      <c r="CG8" s="72"/>
+      <c r="CH8" s="72"/>
+      <c r="CI8" s="72"/>
+      <c r="CJ8" s="72"/>
+      <c r="CK8" s="72"/>
+      <c r="CL8" s="72"/>
+      <c r="CM8" s="72"/>
+      <c r="CN8" s="72"/>
+      <c r="CO8" s="72"/>
+      <c r="CP8" s="72"/>
+      <c r="CQ8" s="72"/>
+      <c r="CR8" s="72"/>
+      <c r="CS8" s="72"/>
+      <c r="CT8" s="72"/>
+      <c r="CU8" s="72"/>
+      <c r="CV8" s="72"/>
+      <c r="CW8" s="72"/>
+      <c r="CX8" s="72"/>
+      <c r="CY8" s="72"/>
+      <c r="CZ8" s="72"/>
+      <c r="DA8" s="72"/>
+      <c r="DB8" s="72"/>
+      <c r="DC8" s="72"/>
+      <c r="DD8" s="72"/>
+      <c r="DE8" s="72"/>
+      <c r="DF8" s="72"/>
+      <c r="DG8" s="72"/>
+      <c r="DH8" s="72"/>
+      <c r="DI8" s="72"/>
+      <c r="DJ8" s="72"/>
+      <c r="DK8" s="72"/>
+      <c r="DL8" s="72"/>
+      <c r="DM8" s="72"/>
+      <c r="DN8" s="72"/>
+      <c r="DO8" s="72"/>
+      <c r="DP8" s="72"/>
+      <c r="DQ8" s="72"/>
+      <c r="DR8" s="72"/>
+      <c r="DS8" s="72"/>
+      <c r="DT8" s="72"/>
+      <c r="DU8" s="72"/>
+      <c r="DV8" s="72"/>
+      <c r="DW8" s="72"/>
+      <c r="DX8" s="72"/>
+      <c r="DY8" s="72"/>
+      <c r="DZ8" s="72"/>
+      <c r="EA8" s="72"/>
+      <c r="EB8" s="72"/>
+      <c r="EC8" s="72"/>
+      <c r="ED8" s="72"/>
+      <c r="EE8" s="72"/>
+      <c r="EF8" s="72"/>
+      <c r="EG8" s="72"/>
+      <c r="EH8" s="72"/>
+      <c r="EI8" s="72"/>
+      <c r="EJ8" s="72"/>
+      <c r="EK8" s="72"/>
+      <c r="EL8" s="72"/>
+      <c r="EM8" s="72"/>
+      <c r="EN8" s="72"/>
+      <c r="EO8" s="72"/>
+      <c r="EP8" s="72"/>
+      <c r="EQ8" s="72"/>
+      <c r="ER8" s="72"/>
+      <c r="ES8" s="72"/>
+      <c r="ET8" s="72"/>
+      <c r="EU8" s="72"/>
+      <c r="EV8" s="72"/>
+      <c r="EW8" s="72"/>
+      <c r="EX8" s="72"/>
+      <c r="EY8" s="72"/>
+      <c r="EZ8" s="72"/>
+      <c r="FA8" s="72"/>
+      <c r="FB8" s="72"/>
+      <c r="FC8" s="72"/>
+      <c r="FD8" s="72"/>
+      <c r="FE8" s="72"/>
+      <c r="FF8" s="72"/>
+      <c r="FG8" s="72"/>
+      <c r="FH8" s="72"/>
+      <c r="FI8" s="72"/>
+      <c r="FJ8" s="72"/>
+      <c r="FK8" s="72"/>
+      <c r="FL8" s="72"/>
+      <c r="FM8" s="72"/>
+      <c r="FN8" s="72"/>
+      <c r="FO8" s="72"/>
+      <c r="FP8" s="72"/>
+      <c r="FQ8" s="72"/>
+      <c r="FR8" s="72"/>
+      <c r="FS8" s="72"/>
+      <c r="FT8" s="72"/>
+      <c r="FU8" s="72"/>
+      <c r="FV8" s="72"/>
+      <c r="FW8" s="72"/>
+      <c r="FX8" s="72"/>
+      <c r="FY8" s="72"/>
+      <c r="FZ8" s="72"/>
+      <c r="GA8" s="72"/>
+      <c r="GB8" s="72"/>
+      <c r="GC8" s="72"/>
+      <c r="GD8" s="72"/>
+      <c r="GE8" s="72"/>
+      <c r="GF8" s="72"/>
+      <c r="GG8" s="72"/>
+      <c r="GH8" s="72"/>
+      <c r="GI8" s="72"/>
+      <c r="GJ8" s="72"/>
+      <c r="GK8" s="72"/>
+      <c r="GL8" s="72"/>
+      <c r="GM8" s="72"/>
+      <c r="GN8" s="72"/>
+      <c r="GO8" s="72"/>
+      <c r="GP8" s="72"/>
+      <c r="GQ8" s="72"/>
+      <c r="GR8" s="72"/>
+      <c r="GS8" s="72"/>
+      <c r="GT8" s="72"/>
+      <c r="GU8" s="72"/>
+      <c r="GV8" s="72"/>
+      <c r="GW8" s="72"/>
+      <c r="GX8" s="72"/>
+      <c r="GY8" s="72"/>
+      <c r="GZ8" s="72"/>
+      <c r="HA8" s="72"/>
+      <c r="HB8" s="72"/>
+      <c r="HC8" s="73"/>
     </row>
     <row r="9" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
@@ -3340,7 +3343,7 @@
       <c r="G9" s="33"/>
       <c r="H9" s="34"/>
       <c r="I9" s="46"/>
-      <c r="J9" s="70"/>
+      <c r="J9" s="69"/>
     </row>
     <row r="10" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
@@ -3351,7 +3354,7 @@
       <c r="G10" s="33"/>
       <c r="H10" s="34"/>
       <c r="I10" s="46"/>
-      <c r="J10" s="70"/>
+      <c r="J10" s="69"/>
     </row>
     <row r="11" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
@@ -3362,7 +3365,7 @@
       <c r="G11" s="33"/>
       <c r="H11" s="34"/>
       <c r="I11" s="46"/>
-      <c r="J11" s="70"/>
+      <c r="J11" s="69"/>
     </row>
     <row r="12" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
@@ -3373,7 +3376,7 @@
       <c r="G12" s="33"/>
       <c r="H12" s="34"/>
       <c r="I12" s="46"/>
-      <c r="J12" s="70"/>
+      <c r="J12" s="69"/>
     </row>
     <row r="13" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B13" s="32"/>
@@ -3384,7 +3387,7 @@
       <c r="G13" s="33"/>
       <c r="H13" s="34"/>
       <c r="I13" s="46"/>
-      <c r="J13" s="70"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
@@ -3395,7 +3398,7 @@
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
       <c r="I14" s="46"/>
-      <c r="J14" s="70"/>
+      <c r="J14" s="69"/>
     </row>
     <row r="15" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
@@ -3406,7 +3409,7 @@
       <c r="G15" s="33"/>
       <c r="H15" s="34"/>
       <c r="I15" s="46"/>
-      <c r="J15" s="70"/>
+      <c r="J15" s="69"/>
     </row>
     <row r="16" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
@@ -3417,7 +3420,7 @@
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
       <c r="I16" s="46"/>
-      <c r="J16" s="70"/>
+      <c r="J16" s="69"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
@@ -3428,7 +3431,7 @@
       <c r="G17" s="33"/>
       <c r="H17" s="34"/>
       <c r="I17" s="46"/>
-      <c r="J17" s="70"/>
+      <c r="J17" s="69"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
@@ -3439,7 +3442,7 @@
       <c r="G18" s="33"/>
       <c r="H18" s="34"/>
       <c r="I18" s="46"/>
-      <c r="J18" s="70"/>
+      <c r="J18" s="69"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
@@ -3450,7 +3453,7 @@
       <c r="G19" s="33"/>
       <c r="H19" s="34"/>
       <c r="I19" s="46"/>
-      <c r="J19" s="70"/>
+      <c r="J19" s="69"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
@@ -3461,7 +3464,7 @@
       <c r="G20" s="33"/>
       <c r="H20" s="34"/>
       <c r="I20" s="46"/>
-      <c r="J20" s="70"/>
+      <c r="J20" s="69"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
@@ -3472,7 +3475,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="34"/>
       <c r="I21" s="46"/>
-      <c r="J21" s="70"/>
+      <c r="J21" s="69"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
@@ -3483,7 +3486,7 @@
       <c r="G22" s="33"/>
       <c r="H22" s="34"/>
       <c r="I22" s="46"/>
-      <c r="J22" s="70"/>
+      <c r="J22" s="69"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
@@ -3494,7 +3497,7 @@
       <c r="G23" s="33"/>
       <c r="H23" s="34"/>
       <c r="I23" s="46"/>
-      <c r="J23" s="70"/>
+      <c r="J23" s="69"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
@@ -3505,7 +3508,7 @@
       <c r="G24" s="33"/>
       <c r="H24" s="34"/>
       <c r="I24" s="46"/>
-      <c r="J24" s="70"/>
+      <c r="J24" s="69"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
@@ -3516,7 +3519,7 @@
       <c r="G25" s="33"/>
       <c r="H25" s="34"/>
       <c r="I25" s="46"/>
-      <c r="J25" s="70"/>
+      <c r="J25" s="69"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
@@ -3527,7 +3530,7 @@
       <c r="G26" s="33"/>
       <c r="H26" s="34"/>
       <c r="I26" s="46"/>
-      <c r="J26" s="70"/>
+      <c r="J26" s="69"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
@@ -3538,7 +3541,7 @@
       <c r="G27" s="33"/>
       <c r="H27" s="34"/>
       <c r="I27" s="46"/>
-      <c r="J27" s="70"/>
+      <c r="J27" s="69"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
@@ -3549,7 +3552,7 @@
       <c r="G28" s="33"/>
       <c r="H28" s="34"/>
       <c r="I28" s="46"/>
-      <c r="J28" s="70"/>
+      <c r="J28" s="69"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
@@ -3560,7 +3563,7 @@
       <c r="G29" s="33"/>
       <c r="H29" s="34"/>
       <c r="I29" s="46"/>
-      <c r="J29" s="70"/>
+      <c r="J29" s="69"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
@@ -3571,7 +3574,7 @@
       <c r="G30" s="33"/>
       <c r="H30" s="34"/>
       <c r="I30" s="46"/>
-      <c r="J30" s="70"/>
+      <c r="J30" s="69"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="32"/>
@@ -3582,7 +3585,7 @@
       <c r="G31" s="33"/>
       <c r="H31" s="34"/>
       <c r="I31" s="46"/>
-      <c r="J31" s="70"/>
+      <c r="J31" s="69"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
@@ -3593,7 +3596,7 @@
       <c r="G32" s="33"/>
       <c r="H32" s="34"/>
       <c r="I32" s="46"/>
-      <c r="J32" s="70"/>
+      <c r="J32" s="69"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
@@ -3604,7 +3607,7 @@
       <c r="G33" s="33"/>
       <c r="H33" s="34"/>
       <c r="I33" s="46"/>
-      <c r="J33" s="70"/>
+      <c r="J33" s="69"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
@@ -3615,7 +3618,7 @@
       <c r="G34" s="33"/>
       <c r="H34" s="34"/>
       <c r="I34" s="46"/>
-      <c r="J34" s="70"/>
+      <c r="J34" s="69"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="32"/>
@@ -3626,7 +3629,7 @@
       <c r="G35" s="33"/>
       <c r="H35" s="34"/>
       <c r="I35" s="46"/>
-      <c r="J35" s="70"/>
+      <c r="J35" s="69"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
@@ -3637,7 +3640,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="34"/>
       <c r="I36" s="46"/>
-      <c r="J36" s="70"/>
+      <c r="J36" s="69"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
@@ -3648,7 +3651,7 @@
       <c r="G37" s="33"/>
       <c r="H37" s="34"/>
       <c r="I37" s="46"/>
-      <c r="J37" s="70"/>
+      <c r="J37" s="69"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="32"/>
@@ -3659,7 +3662,7 @@
       <c r="G38" s="33"/>
       <c r="H38" s="34"/>
       <c r="I38" s="46"/>
-      <c r="J38" s="70"/>
+      <c r="J38" s="69"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="32"/>
@@ -3670,7 +3673,7 @@
       <c r="G39" s="33"/>
       <c r="H39" s="34"/>
       <c r="I39" s="46"/>
-      <c r="J39" s="70"/>
+      <c r="J39" s="69"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
@@ -3681,7 +3684,7 @@
       <c r="G40" s="33"/>
       <c r="H40" s="34"/>
       <c r="I40" s="46"/>
-      <c r="J40" s="70"/>
+      <c r="J40" s="69"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
@@ -3692,7 +3695,7 @@
       <c r="G41" s="33"/>
       <c r="H41" s="34"/>
       <c r="I41" s="46"/>
-      <c r="J41" s="70"/>
+      <c r="J41" s="69"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
@@ -3703,7 +3706,7 @@
       <c r="G42" s="33"/>
       <c r="H42" s="34"/>
       <c r="I42" s="46"/>
-      <c r="J42" s="70"/>
+      <c r="J42" s="69"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
@@ -3714,7 +3717,7 @@
       <c r="G43" s="33"/>
       <c r="H43" s="34"/>
       <c r="I43" s="46"/>
-      <c r="J43" s="70"/>
+      <c r="J43" s="69"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
@@ -3725,7 +3728,7 @@
       <c r="G44" s="33"/>
       <c r="H44" s="34"/>
       <c r="I44" s="46"/>
-      <c r="J44" s="70"/>
+      <c r="J44" s="69"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
@@ -3736,7 +3739,7 @@
       <c r="G45" s="33"/>
       <c r="H45" s="34"/>
       <c r="I45" s="46"/>
-      <c r="J45" s="70"/>
+      <c r="J45" s="69"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
@@ -3747,7 +3750,7 @@
       <c r="G46" s="33"/>
       <c r="H46" s="34"/>
       <c r="I46" s="46"/>
-      <c r="J46" s="70"/>
+      <c r="J46" s="69"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="32"/>
@@ -3758,7 +3761,7 @@
       <c r="G47" s="33"/>
       <c r="H47" s="34"/>
       <c r="I47" s="46"/>
-      <c r="J47" s="70"/>
+      <c r="J47" s="69"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
@@ -3769,7 +3772,7 @@
       <c r="G48" s="33"/>
       <c r="H48" s="34"/>
       <c r="I48" s="46"/>
-      <c r="J48" s="70"/>
+      <c r="J48" s="69"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="32"/>
@@ -3780,7 +3783,7 @@
       <c r="G49" s="33"/>
       <c r="H49" s="34"/>
       <c r="I49" s="46"/>
-      <c r="J49" s="70"/>
+      <c r="J49" s="69"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="32"/>
@@ -3791,7 +3794,7 @@
       <c r="G50" s="33"/>
       <c r="H50" s="34"/>
       <c r="I50" s="46"/>
-      <c r="J50" s="70"/>
+      <c r="J50" s="69"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="32"/>
@@ -3802,7 +3805,7 @@
       <c r="G51" s="33"/>
       <c r="H51" s="34"/>
       <c r="I51" s="46"/>
-      <c r="J51" s="70"/>
+      <c r="J51" s="69"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="32"/>
@@ -3813,7 +3816,7 @@
       <c r="G52" s="33"/>
       <c r="H52" s="34"/>
       <c r="I52" s="46"/>
-      <c r="J52" s="70"/>
+      <c r="J52" s="69"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="32"/>
@@ -3824,7 +3827,7 @@
       <c r="G53" s="33"/>
       <c r="H53" s="34"/>
       <c r="I53" s="46"/>
-      <c r="J53" s="70"/>
+      <c r="J53" s="69"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="32"/>
@@ -3835,7 +3838,7 @@
       <c r="G54" s="33"/>
       <c r="H54" s="34"/>
       <c r="I54" s="46"/>
-      <c r="J54" s="70"/>
+      <c r="J54" s="69"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="32"/>
@@ -3846,7 +3849,7 @@
       <c r="G55" s="33"/>
       <c r="H55" s="34"/>
       <c r="I55" s="46"/>
-      <c r="J55" s="70"/>
+      <c r="J55" s="69"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="32"/>
@@ -3857,7 +3860,7 @@
       <c r="G56" s="33"/>
       <c r="H56" s="34"/>
       <c r="I56" s="46"/>
-      <c r="J56" s="70"/>
+      <c r="J56" s="69"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="32"/>
@@ -3868,7 +3871,7 @@
       <c r="G57" s="33"/>
       <c r="H57" s="34"/>
       <c r="I57" s="32"/>
-      <c r="J57" s="70"/>
+      <c r="J57" s="69"/>
     </row>
     <row r="1048575" spans="12:211" x14ac:dyDescent="0.25">
       <c r="L1048575" s="48"/>

</xml_diff>

<commit_message>
Fixing 'Type of data' field, other fixes
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1DI.xlsx
+++ b/form_reporting_templates/Form-1DI.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7C7E6-32F4-4A4D-A566-5AB77EA5C761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573E9586-D763-4542-80C2-C848C92C0A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -959,10 +959,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1036,6 +1032,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1138,7 +1137,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="112" t="s">
+      <c r="C20" s="78" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="40"/>
@@ -1763,11 +1763,8 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="B2:H3"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19" xr:uid="{B9CB61C8-BBA2-4A24-8E84-84C263F59204}">
-      <formula1>"&lt;0&gt;0"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20" xr:uid="{84E8478B-349E-439F-A70D-E4E827D455F5}">
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C20" xr:uid="{B9CB61C8-BBA2-4A24-8E84-84C263F59204}">
       <formula1>"&lt;0&gt;0"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1794,19 +1791,19 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="64" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="65" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="65" customWidth="1"/>
-    <col min="5" max="5" width="14" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="64" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="65" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="67" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="64" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="70" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="78" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="74"/>
-    <col min="13" max="210" width="9.140625" style="75"/>
-    <col min="211" max="211" width="9.140625" style="76"/>
+    <col min="2" max="2" width="11.42578125" style="63" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="64" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="64" customWidth="1"/>
+    <col min="5" max="5" width="14" style="65" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="63" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="64" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="66" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="63" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="69" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="77" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="73"/>
+    <col min="13" max="210" width="9.140625" style="74"/>
+    <col min="211" max="211" width="9.140625" style="75"/>
     <col min="212" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
@@ -2258,7 +2255,7 @@
         <v>18</v>
       </c>
       <c r="J4" s="100"/>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="61" t="s">
         <v>12</v>
       </c>
       <c r="L4" s="26"/>
@@ -2903,7 +2900,7 @@
       <c r="E7" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="112" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="57" t="s">
@@ -2912,13 +2909,13 @@
       <c r="H7" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="60" t="s">
+      <c r="I7" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="61" t="s">
+      <c r="J7" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="63" t="s">
+      <c r="K7" s="62" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="29"/>
@@ -3131,208 +3128,208 @@
       <c r="G8" s="43"/>
       <c r="H8" s="44"/>
       <c r="I8" s="45"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
-      <c r="R8" s="72"/>
-      <c r="S8" s="72"/>
-      <c r="T8" s="72"/>
-      <c r="U8" s="72"/>
-      <c r="V8" s="72"/>
-      <c r="W8" s="72"/>
-      <c r="X8" s="72"/>
-      <c r="Y8" s="72"/>
-      <c r="Z8" s="72"/>
-      <c r="AA8" s="72"/>
-      <c r="AB8" s="72"/>
-      <c r="AC8" s="72"/>
-      <c r="AD8" s="72"/>
-      <c r="AE8" s="72"/>
-      <c r="AF8" s="72"/>
-      <c r="AG8" s="72"/>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="72"/>
-      <c r="AJ8" s="72"/>
-      <c r="AK8" s="72"/>
-      <c r="AL8" s="72"/>
-      <c r="AM8" s="72"/>
-      <c r="AN8" s="72"/>
-      <c r="AO8" s="72"/>
-      <c r="AP8" s="72"/>
-      <c r="AQ8" s="72"/>
-      <c r="AR8" s="72"/>
-      <c r="AS8" s="72"/>
-      <c r="AT8" s="72"/>
-      <c r="AU8" s="72"/>
-      <c r="AV8" s="72"/>
-      <c r="AW8" s="72"/>
-      <c r="AX8" s="72"/>
-      <c r="AY8" s="72"/>
-      <c r="AZ8" s="72"/>
-      <c r="BA8" s="72"/>
-      <c r="BB8" s="72"/>
-      <c r="BC8" s="72"/>
-      <c r="BD8" s="72"/>
-      <c r="BE8" s="72"/>
-      <c r="BF8" s="72"/>
-      <c r="BG8" s="72"/>
-      <c r="BH8" s="72"/>
-      <c r="BI8" s="72"/>
-      <c r="BJ8" s="72"/>
-      <c r="BK8" s="72"/>
-      <c r="BL8" s="72"/>
-      <c r="BM8" s="72"/>
-      <c r="BN8" s="72"/>
-      <c r="BO8" s="72"/>
-      <c r="BP8" s="72"/>
-      <c r="BQ8" s="72"/>
-      <c r="BR8" s="72"/>
-      <c r="BS8" s="72"/>
-      <c r="BT8" s="72"/>
-      <c r="BU8" s="72"/>
-      <c r="BV8" s="72"/>
-      <c r="BW8" s="72"/>
-      <c r="BX8" s="72"/>
-      <c r="BY8" s="72"/>
-      <c r="BZ8" s="72"/>
-      <c r="CA8" s="72"/>
-      <c r="CB8" s="72"/>
-      <c r="CC8" s="72"/>
-      <c r="CD8" s="72"/>
-      <c r="CE8" s="72"/>
-      <c r="CF8" s="72"/>
-      <c r="CG8" s="72"/>
-      <c r="CH8" s="72"/>
-      <c r="CI8" s="72"/>
-      <c r="CJ8" s="72"/>
-      <c r="CK8" s="72"/>
-      <c r="CL8" s="72"/>
-      <c r="CM8" s="72"/>
-      <c r="CN8" s="72"/>
-      <c r="CO8" s="72"/>
-      <c r="CP8" s="72"/>
-      <c r="CQ8" s="72"/>
-      <c r="CR8" s="72"/>
-      <c r="CS8" s="72"/>
-      <c r="CT8" s="72"/>
-      <c r="CU8" s="72"/>
-      <c r="CV8" s="72"/>
-      <c r="CW8" s="72"/>
-      <c r="CX8" s="72"/>
-      <c r="CY8" s="72"/>
-      <c r="CZ8" s="72"/>
-      <c r="DA8" s="72"/>
-      <c r="DB8" s="72"/>
-      <c r="DC8" s="72"/>
-      <c r="DD8" s="72"/>
-      <c r="DE8" s="72"/>
-      <c r="DF8" s="72"/>
-      <c r="DG8" s="72"/>
-      <c r="DH8" s="72"/>
-      <c r="DI8" s="72"/>
-      <c r="DJ8" s="72"/>
-      <c r="DK8" s="72"/>
-      <c r="DL8" s="72"/>
-      <c r="DM8" s="72"/>
-      <c r="DN8" s="72"/>
-      <c r="DO8" s="72"/>
-      <c r="DP8" s="72"/>
-      <c r="DQ8" s="72"/>
-      <c r="DR8" s="72"/>
-      <c r="DS8" s="72"/>
-      <c r="DT8" s="72"/>
-      <c r="DU8" s="72"/>
-      <c r="DV8" s="72"/>
-      <c r="DW8" s="72"/>
-      <c r="DX8" s="72"/>
-      <c r="DY8" s="72"/>
-      <c r="DZ8" s="72"/>
-      <c r="EA8" s="72"/>
-      <c r="EB8" s="72"/>
-      <c r="EC8" s="72"/>
-      <c r="ED8" s="72"/>
-      <c r="EE8" s="72"/>
-      <c r="EF8" s="72"/>
-      <c r="EG8" s="72"/>
-      <c r="EH8" s="72"/>
-      <c r="EI8" s="72"/>
-      <c r="EJ8" s="72"/>
-      <c r="EK8" s="72"/>
-      <c r="EL8" s="72"/>
-      <c r="EM8" s="72"/>
-      <c r="EN8" s="72"/>
-      <c r="EO8" s="72"/>
-      <c r="EP8" s="72"/>
-      <c r="EQ8" s="72"/>
-      <c r="ER8" s="72"/>
-      <c r="ES8" s="72"/>
-      <c r="ET8" s="72"/>
-      <c r="EU8" s="72"/>
-      <c r="EV8" s="72"/>
-      <c r="EW8" s="72"/>
-      <c r="EX8" s="72"/>
-      <c r="EY8" s="72"/>
-      <c r="EZ8" s="72"/>
-      <c r="FA8" s="72"/>
-      <c r="FB8" s="72"/>
-      <c r="FC8" s="72"/>
-      <c r="FD8" s="72"/>
-      <c r="FE8" s="72"/>
-      <c r="FF8" s="72"/>
-      <c r="FG8" s="72"/>
-      <c r="FH8" s="72"/>
-      <c r="FI8" s="72"/>
-      <c r="FJ8" s="72"/>
-      <c r="FK8" s="72"/>
-      <c r="FL8" s="72"/>
-      <c r="FM8" s="72"/>
-      <c r="FN8" s="72"/>
-      <c r="FO8" s="72"/>
-      <c r="FP8" s="72"/>
-      <c r="FQ8" s="72"/>
-      <c r="FR8" s="72"/>
-      <c r="FS8" s="72"/>
-      <c r="FT8" s="72"/>
-      <c r="FU8" s="72"/>
-      <c r="FV8" s="72"/>
-      <c r="FW8" s="72"/>
-      <c r="FX8" s="72"/>
-      <c r="FY8" s="72"/>
-      <c r="FZ8" s="72"/>
-      <c r="GA8" s="72"/>
-      <c r="GB8" s="72"/>
-      <c r="GC8" s="72"/>
-      <c r="GD8" s="72"/>
-      <c r="GE8" s="72"/>
-      <c r="GF8" s="72"/>
-      <c r="GG8" s="72"/>
-      <c r="GH8" s="72"/>
-      <c r="GI8" s="72"/>
-      <c r="GJ8" s="72"/>
-      <c r="GK8" s="72"/>
-      <c r="GL8" s="72"/>
-      <c r="GM8" s="72"/>
-      <c r="GN8" s="72"/>
-      <c r="GO8" s="72"/>
-      <c r="GP8" s="72"/>
-      <c r="GQ8" s="72"/>
-      <c r="GR8" s="72"/>
-      <c r="GS8" s="72"/>
-      <c r="GT8" s="72"/>
-      <c r="GU8" s="72"/>
-      <c r="GV8" s="72"/>
-      <c r="GW8" s="72"/>
-      <c r="GX8" s="72"/>
-      <c r="GY8" s="72"/>
-      <c r="GZ8" s="72"/>
-      <c r="HA8" s="72"/>
-      <c r="HB8" s="72"/>
-      <c r="HC8" s="73"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
+      <c r="R8" s="71"/>
+      <c r="S8" s="71"/>
+      <c r="T8" s="71"/>
+      <c r="U8" s="71"/>
+      <c r="V8" s="71"/>
+      <c r="W8" s="71"/>
+      <c r="X8" s="71"/>
+      <c r="Y8" s="71"/>
+      <c r="Z8" s="71"/>
+      <c r="AA8" s="71"/>
+      <c r="AB8" s="71"/>
+      <c r="AC8" s="71"/>
+      <c r="AD8" s="71"/>
+      <c r="AE8" s="71"/>
+      <c r="AF8" s="71"/>
+      <c r="AG8" s="71"/>
+      <c r="AH8" s="71"/>
+      <c r="AI8" s="71"/>
+      <c r="AJ8" s="71"/>
+      <c r="AK8" s="71"/>
+      <c r="AL8" s="71"/>
+      <c r="AM8" s="71"/>
+      <c r="AN8" s="71"/>
+      <c r="AO8" s="71"/>
+      <c r="AP8" s="71"/>
+      <c r="AQ8" s="71"/>
+      <c r="AR8" s="71"/>
+      <c r="AS8" s="71"/>
+      <c r="AT8" s="71"/>
+      <c r="AU8" s="71"/>
+      <c r="AV8" s="71"/>
+      <c r="AW8" s="71"/>
+      <c r="AX8" s="71"/>
+      <c r="AY8" s="71"/>
+      <c r="AZ8" s="71"/>
+      <c r="BA8" s="71"/>
+      <c r="BB8" s="71"/>
+      <c r="BC8" s="71"/>
+      <c r="BD8" s="71"/>
+      <c r="BE8" s="71"/>
+      <c r="BF8" s="71"/>
+      <c r="BG8" s="71"/>
+      <c r="BH8" s="71"/>
+      <c r="BI8" s="71"/>
+      <c r="BJ8" s="71"/>
+      <c r="BK8" s="71"/>
+      <c r="BL8" s="71"/>
+      <c r="BM8" s="71"/>
+      <c r="BN8" s="71"/>
+      <c r="BO8" s="71"/>
+      <c r="BP8" s="71"/>
+      <c r="BQ8" s="71"/>
+      <c r="BR8" s="71"/>
+      <c r="BS8" s="71"/>
+      <c r="BT8" s="71"/>
+      <c r="BU8" s="71"/>
+      <c r="BV8" s="71"/>
+      <c r="BW8" s="71"/>
+      <c r="BX8" s="71"/>
+      <c r="BY8" s="71"/>
+      <c r="BZ8" s="71"/>
+      <c r="CA8" s="71"/>
+      <c r="CB8" s="71"/>
+      <c r="CC8" s="71"/>
+      <c r="CD8" s="71"/>
+      <c r="CE8" s="71"/>
+      <c r="CF8" s="71"/>
+      <c r="CG8" s="71"/>
+      <c r="CH8" s="71"/>
+      <c r="CI8" s="71"/>
+      <c r="CJ8" s="71"/>
+      <c r="CK8" s="71"/>
+      <c r="CL8" s="71"/>
+      <c r="CM8" s="71"/>
+      <c r="CN8" s="71"/>
+      <c r="CO8" s="71"/>
+      <c r="CP8" s="71"/>
+      <c r="CQ8" s="71"/>
+      <c r="CR8" s="71"/>
+      <c r="CS8" s="71"/>
+      <c r="CT8" s="71"/>
+      <c r="CU8" s="71"/>
+      <c r="CV8" s="71"/>
+      <c r="CW8" s="71"/>
+      <c r="CX8" s="71"/>
+      <c r="CY8" s="71"/>
+      <c r="CZ8" s="71"/>
+      <c r="DA8" s="71"/>
+      <c r="DB8" s="71"/>
+      <c r="DC8" s="71"/>
+      <c r="DD8" s="71"/>
+      <c r="DE8" s="71"/>
+      <c r="DF8" s="71"/>
+      <c r="DG8" s="71"/>
+      <c r="DH8" s="71"/>
+      <c r="DI8" s="71"/>
+      <c r="DJ8" s="71"/>
+      <c r="DK8" s="71"/>
+      <c r="DL8" s="71"/>
+      <c r="DM8" s="71"/>
+      <c r="DN8" s="71"/>
+      <c r="DO8" s="71"/>
+      <c r="DP8" s="71"/>
+      <c r="DQ8" s="71"/>
+      <c r="DR8" s="71"/>
+      <c r="DS8" s="71"/>
+      <c r="DT8" s="71"/>
+      <c r="DU8" s="71"/>
+      <c r="DV8" s="71"/>
+      <c r="DW8" s="71"/>
+      <c r="DX8" s="71"/>
+      <c r="DY8" s="71"/>
+      <c r="DZ8" s="71"/>
+      <c r="EA8" s="71"/>
+      <c r="EB8" s="71"/>
+      <c r="EC8" s="71"/>
+      <c r="ED8" s="71"/>
+      <c r="EE8" s="71"/>
+      <c r="EF8" s="71"/>
+      <c r="EG8" s="71"/>
+      <c r="EH8" s="71"/>
+      <c r="EI8" s="71"/>
+      <c r="EJ8" s="71"/>
+      <c r="EK8" s="71"/>
+      <c r="EL8" s="71"/>
+      <c r="EM8" s="71"/>
+      <c r="EN8" s="71"/>
+      <c r="EO8" s="71"/>
+      <c r="EP8" s="71"/>
+      <c r="EQ8" s="71"/>
+      <c r="ER8" s="71"/>
+      <c r="ES8" s="71"/>
+      <c r="ET8" s="71"/>
+      <c r="EU8" s="71"/>
+      <c r="EV8" s="71"/>
+      <c r="EW8" s="71"/>
+      <c r="EX8" s="71"/>
+      <c r="EY8" s="71"/>
+      <c r="EZ8" s="71"/>
+      <c r="FA8" s="71"/>
+      <c r="FB8" s="71"/>
+      <c r="FC8" s="71"/>
+      <c r="FD8" s="71"/>
+      <c r="FE8" s="71"/>
+      <c r="FF8" s="71"/>
+      <c r="FG8" s="71"/>
+      <c r="FH8" s="71"/>
+      <c r="FI8" s="71"/>
+      <c r="FJ8" s="71"/>
+      <c r="FK8" s="71"/>
+      <c r="FL8" s="71"/>
+      <c r="FM8" s="71"/>
+      <c r="FN8" s="71"/>
+      <c r="FO8" s="71"/>
+      <c r="FP8" s="71"/>
+      <c r="FQ8" s="71"/>
+      <c r="FR8" s="71"/>
+      <c r="FS8" s="71"/>
+      <c r="FT8" s="71"/>
+      <c r="FU8" s="71"/>
+      <c r="FV8" s="71"/>
+      <c r="FW8" s="71"/>
+      <c r="FX8" s="71"/>
+      <c r="FY8" s="71"/>
+      <c r="FZ8" s="71"/>
+      <c r="GA8" s="71"/>
+      <c r="GB8" s="71"/>
+      <c r="GC8" s="71"/>
+      <c r="GD8" s="71"/>
+      <c r="GE8" s="71"/>
+      <c r="GF8" s="71"/>
+      <c r="GG8" s="71"/>
+      <c r="GH8" s="71"/>
+      <c r="GI8" s="71"/>
+      <c r="GJ8" s="71"/>
+      <c r="GK8" s="71"/>
+      <c r="GL8" s="71"/>
+      <c r="GM8" s="71"/>
+      <c r="GN8" s="71"/>
+      <c r="GO8" s="71"/>
+      <c r="GP8" s="71"/>
+      <c r="GQ8" s="71"/>
+      <c r="GR8" s="71"/>
+      <c r="GS8" s="71"/>
+      <c r="GT8" s="71"/>
+      <c r="GU8" s="71"/>
+      <c r="GV8" s="71"/>
+      <c r="GW8" s="71"/>
+      <c r="GX8" s="71"/>
+      <c r="GY8" s="71"/>
+      <c r="GZ8" s="71"/>
+      <c r="HA8" s="71"/>
+      <c r="HB8" s="71"/>
+      <c r="HC8" s="72"/>
     </row>
     <row r="9" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
@@ -3343,7 +3340,7 @@
       <c r="G9" s="33"/>
       <c r="H9" s="34"/>
       <c r="I9" s="46"/>
-      <c r="J9" s="69"/>
+      <c r="J9" s="68"/>
     </row>
     <row r="10" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
@@ -3354,7 +3351,7 @@
       <c r="G10" s="33"/>
       <c r="H10" s="34"/>
       <c r="I10" s="46"/>
-      <c r="J10" s="69"/>
+      <c r="J10" s="68"/>
     </row>
     <row r="11" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
@@ -3365,7 +3362,7 @@
       <c r="G11" s="33"/>
       <c r="H11" s="34"/>
       <c r="I11" s="46"/>
-      <c r="J11" s="69"/>
+      <c r="J11" s="68"/>
     </row>
     <row r="12" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
@@ -3376,7 +3373,7 @@
       <c r="G12" s="33"/>
       <c r="H12" s="34"/>
       <c r="I12" s="46"/>
-      <c r="J12" s="69"/>
+      <c r="J12" s="68"/>
     </row>
     <row r="13" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B13" s="32"/>
@@ -3387,7 +3384,7 @@
       <c r="G13" s="33"/>
       <c r="H13" s="34"/>
       <c r="I13" s="46"/>
-      <c r="J13" s="69"/>
+      <c r="J13" s="68"/>
     </row>
     <row r="14" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
@@ -3398,7 +3395,7 @@
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
       <c r="I14" s="46"/>
-      <c r="J14" s="69"/>
+      <c r="J14" s="68"/>
     </row>
     <row r="15" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
@@ -3409,7 +3406,7 @@
       <c r="G15" s="33"/>
       <c r="H15" s="34"/>
       <c r="I15" s="46"/>
-      <c r="J15" s="69"/>
+      <c r="J15" s="68"/>
     </row>
     <row r="16" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
@@ -3420,7 +3417,7 @@
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
       <c r="I16" s="46"/>
-      <c r="J16" s="69"/>
+      <c r="J16" s="68"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
@@ -3431,7 +3428,7 @@
       <c r="G17" s="33"/>
       <c r="H17" s="34"/>
       <c r="I17" s="46"/>
-      <c r="J17" s="69"/>
+      <c r="J17" s="68"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
@@ -3442,7 +3439,7 @@
       <c r="G18" s="33"/>
       <c r="H18" s="34"/>
       <c r="I18" s="46"/>
-      <c r="J18" s="69"/>
+      <c r="J18" s="68"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
@@ -3453,7 +3450,7 @@
       <c r="G19" s="33"/>
       <c r="H19" s="34"/>
       <c r="I19" s="46"/>
-      <c r="J19" s="69"/>
+      <c r="J19" s="68"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
@@ -3464,7 +3461,7 @@
       <c r="G20" s="33"/>
       <c r="H20" s="34"/>
       <c r="I20" s="46"/>
-      <c r="J20" s="69"/>
+      <c r="J20" s="68"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
@@ -3475,7 +3472,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="34"/>
       <c r="I21" s="46"/>
-      <c r="J21" s="69"/>
+      <c r="J21" s="68"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
@@ -3486,7 +3483,7 @@
       <c r="G22" s="33"/>
       <c r="H22" s="34"/>
       <c r="I22" s="46"/>
-      <c r="J22" s="69"/>
+      <c r="J22" s="68"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
@@ -3497,7 +3494,7 @@
       <c r="G23" s="33"/>
       <c r="H23" s="34"/>
       <c r="I23" s="46"/>
-      <c r="J23" s="69"/>
+      <c r="J23" s="68"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
@@ -3508,7 +3505,7 @@
       <c r="G24" s="33"/>
       <c r="H24" s="34"/>
       <c r="I24" s="46"/>
-      <c r="J24" s="69"/>
+      <c r="J24" s="68"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
@@ -3519,7 +3516,7 @@
       <c r="G25" s="33"/>
       <c r="H25" s="34"/>
       <c r="I25" s="46"/>
-      <c r="J25" s="69"/>
+      <c r="J25" s="68"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
@@ -3530,7 +3527,7 @@
       <c r="G26" s="33"/>
       <c r="H26" s="34"/>
       <c r="I26" s="46"/>
-      <c r="J26" s="69"/>
+      <c r="J26" s="68"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
@@ -3541,7 +3538,7 @@
       <c r="G27" s="33"/>
       <c r="H27" s="34"/>
       <c r="I27" s="46"/>
-      <c r="J27" s="69"/>
+      <c r="J27" s="68"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
@@ -3552,7 +3549,7 @@
       <c r="G28" s="33"/>
       <c r="H28" s="34"/>
       <c r="I28" s="46"/>
-      <c r="J28" s="69"/>
+      <c r="J28" s="68"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
@@ -3563,7 +3560,7 @@
       <c r="G29" s="33"/>
       <c r="H29" s="34"/>
       <c r="I29" s="46"/>
-      <c r="J29" s="69"/>
+      <c r="J29" s="68"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
@@ -3574,7 +3571,7 @@
       <c r="G30" s="33"/>
       <c r="H30" s="34"/>
       <c r="I30" s="46"/>
-      <c r="J30" s="69"/>
+      <c r="J30" s="68"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="32"/>
@@ -3585,7 +3582,7 @@
       <c r="G31" s="33"/>
       <c r="H31" s="34"/>
       <c r="I31" s="46"/>
-      <c r="J31" s="69"/>
+      <c r="J31" s="68"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
@@ -3596,7 +3593,7 @@
       <c r="G32" s="33"/>
       <c r="H32" s="34"/>
       <c r="I32" s="46"/>
-      <c r="J32" s="69"/>
+      <c r="J32" s="68"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
@@ -3607,7 +3604,7 @@
       <c r="G33" s="33"/>
       <c r="H33" s="34"/>
       <c r="I33" s="46"/>
-      <c r="J33" s="69"/>
+      <c r="J33" s="68"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
@@ -3618,7 +3615,7 @@
       <c r="G34" s="33"/>
       <c r="H34" s="34"/>
       <c r="I34" s="46"/>
-      <c r="J34" s="69"/>
+      <c r="J34" s="68"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="32"/>
@@ -3629,7 +3626,7 @@
       <c r="G35" s="33"/>
       <c r="H35" s="34"/>
       <c r="I35" s="46"/>
-      <c r="J35" s="69"/>
+      <c r="J35" s="68"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
@@ -3640,7 +3637,7 @@
       <c r="G36" s="33"/>
       <c r="H36" s="34"/>
       <c r="I36" s="46"/>
-      <c r="J36" s="69"/>
+      <c r="J36" s="68"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
@@ -3651,7 +3648,7 @@
       <c r="G37" s="33"/>
       <c r="H37" s="34"/>
       <c r="I37" s="46"/>
-      <c r="J37" s="69"/>
+      <c r="J37" s="68"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="32"/>
@@ -3662,7 +3659,7 @@
       <c r="G38" s="33"/>
       <c r="H38" s="34"/>
       <c r="I38" s="46"/>
-      <c r="J38" s="69"/>
+      <c r="J38" s="68"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="32"/>
@@ -3673,7 +3670,7 @@
       <c r="G39" s="33"/>
       <c r="H39" s="34"/>
       <c r="I39" s="46"/>
-      <c r="J39" s="69"/>
+      <c r="J39" s="68"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
@@ -3684,7 +3681,7 @@
       <c r="G40" s="33"/>
       <c r="H40" s="34"/>
       <c r="I40" s="46"/>
-      <c r="J40" s="69"/>
+      <c r="J40" s="68"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
@@ -3695,7 +3692,7 @@
       <c r="G41" s="33"/>
       <c r="H41" s="34"/>
       <c r="I41" s="46"/>
-      <c r="J41" s="69"/>
+      <c r="J41" s="68"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
@@ -3706,7 +3703,7 @@
       <c r="G42" s="33"/>
       <c r="H42" s="34"/>
       <c r="I42" s="46"/>
-      <c r="J42" s="69"/>
+      <c r="J42" s="68"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
@@ -3717,7 +3714,7 @@
       <c r="G43" s="33"/>
       <c r="H43" s="34"/>
       <c r="I43" s="46"/>
-      <c r="J43" s="69"/>
+      <c r="J43" s="68"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
@@ -3728,7 +3725,7 @@
       <c r="G44" s="33"/>
       <c r="H44" s="34"/>
       <c r="I44" s="46"/>
-      <c r="J44" s="69"/>
+      <c r="J44" s="68"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
@@ -3739,7 +3736,7 @@
       <c r="G45" s="33"/>
       <c r="H45" s="34"/>
       <c r="I45" s="46"/>
-      <c r="J45" s="69"/>
+      <c r="J45" s="68"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
@@ -3750,7 +3747,7 @@
       <c r="G46" s="33"/>
       <c r="H46" s="34"/>
       <c r="I46" s="46"/>
-      <c r="J46" s="69"/>
+      <c r="J46" s="68"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="32"/>
@@ -3761,7 +3758,7 @@
       <c r="G47" s="33"/>
       <c r="H47" s="34"/>
       <c r="I47" s="46"/>
-      <c r="J47" s="69"/>
+      <c r="J47" s="68"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
@@ -3772,7 +3769,7 @@
       <c r="G48" s="33"/>
       <c r="H48" s="34"/>
       <c r="I48" s="46"/>
-      <c r="J48" s="69"/>
+      <c r="J48" s="68"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="32"/>
@@ -3783,7 +3780,7 @@
       <c r="G49" s="33"/>
       <c r="H49" s="34"/>
       <c r="I49" s="46"/>
-      <c r="J49" s="69"/>
+      <c r="J49" s="68"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="32"/>
@@ -3794,7 +3791,7 @@
       <c r="G50" s="33"/>
       <c r="H50" s="34"/>
       <c r="I50" s="46"/>
-      <c r="J50" s="69"/>
+      <c r="J50" s="68"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="32"/>
@@ -3805,7 +3802,7 @@
       <c r="G51" s="33"/>
       <c r="H51" s="34"/>
       <c r="I51" s="46"/>
-      <c r="J51" s="69"/>
+      <c r="J51" s="68"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="32"/>
@@ -3816,7 +3813,7 @@
       <c r="G52" s="33"/>
       <c r="H52" s="34"/>
       <c r="I52" s="46"/>
-      <c r="J52" s="69"/>
+      <c r="J52" s="68"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="32"/>
@@ -3827,7 +3824,7 @@
       <c r="G53" s="33"/>
       <c r="H53" s="34"/>
       <c r="I53" s="46"/>
-      <c r="J53" s="69"/>
+      <c r="J53" s="68"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="32"/>
@@ -3838,7 +3835,7 @@
       <c r="G54" s="33"/>
       <c r="H54" s="34"/>
       <c r="I54" s="46"/>
-      <c r="J54" s="69"/>
+      <c r="J54" s="68"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="32"/>
@@ -3849,7 +3846,7 @@
       <c r="G55" s="33"/>
       <c r="H55" s="34"/>
       <c r="I55" s="46"/>
-      <c r="J55" s="69"/>
+      <c r="J55" s="68"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="32"/>
@@ -3860,7 +3857,7 @@
       <c r="G56" s="33"/>
       <c r="H56" s="34"/>
       <c r="I56" s="46"/>
-      <c r="J56" s="69"/>
+      <c r="J56" s="68"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="32"/>
@@ -3871,7 +3868,7 @@
       <c r="G57" s="33"/>
       <c r="H57" s="34"/>
       <c r="I57" s="32"/>
-      <c r="J57" s="69"/>
+      <c r="J57" s="68"/>
     </row>
     <row r="1048575" spans="12:211" x14ac:dyDescent="0.25">
       <c r="L1048575" s="48"/>
@@ -4076,7 +4073,7 @@
       <c r="HC1048575" s="47"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KZ25CrtIDjbQU4RlUR525/jC1mr8ZthrIajwJfoXSGd0RkqL2wIfofqkMs0KBEMEEG9xps/i7/cyguoYLK7ZIw==" saltValue="s47uT0okwH64pvR2SJz+KQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="GZrKIrqnpAc6NX5OZ2neCpMXMDVf/SA7eF5KW7FXmzSsOAKoMj+t2oDjDjVL2ryevIUDA+H1TPHIrcz4oWzhFg==" saltValue="vkusKh8xY+iml5BT24wx8Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B4:E6"/>
     <mergeCell ref="F4:H6"/>

</xml_diff>

<commit_message>
Implementing changes to the forms.
These include:

* Renaming 'Main stratum' as 'Main elements'
* Moving 'Estimation' under 'Original data' (3CE / 4SF)
* Replace onboard processing with onboard storage in Form 2FC
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1DI.xlsx
+++ b/form_reporting_templates/Form-1DI.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573E9586-D763-4542-80C2-C848C92C0A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379A498E-36BB-481D-93EC-DC2A5A54638A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>Main stratum</t>
-  </si>
-  <si>
     <t>IOTC area</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>Flag state</t>
+  </si>
+  <si>
+    <t>Main elements</t>
   </si>
 </sst>
 </file>
@@ -1035,6 +1035,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1136,10 +1140,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1489,24 +1489,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="83" t="s">
-        <v>32</v>
+      <c r="B2" s="84" t="s">
+        <v>31</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="88"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="89"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1514,14 +1514,14 @@
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1556,15 +1556,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="82"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="82" t="s">
-        <v>27</v>
+      <c r="F8" s="83" t="s">
+        <v>26</v>
       </c>
-      <c r="G8" s="82"/>
+      <c r="G8" s="83"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1583,12 +1583,12 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="11"/>
@@ -1605,7 +1605,7 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="10"/>
@@ -1676,7 +1676,7 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="10"/>
@@ -1687,7 +1687,7 @@
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="78" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="40"/>
       <c r="E20" s="10"/>
@@ -1735,11 +1735,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1811,18 +1811,18 @@
       <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="83" t="s">
-        <v>33</v>
+      <c r="B2" s="84" t="s">
+        <v>32</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="110"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="111"/>
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
@@ -2026,235 +2026,235 @@
     </row>
     <row r="3" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="107" t="s">
-        <v>26</v>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="108" t="s">
+        <v>25</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108"/>
-      <c r="X3" s="108"/>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="108"/>
-      <c r="AA3" s="108"/>
-      <c r="AB3" s="108"/>
-      <c r="AC3" s="108"/>
-      <c r="AD3" s="108"/>
-      <c r="AE3" s="108"/>
-      <c r="AF3" s="108"/>
-      <c r="AG3" s="108"/>
-      <c r="AH3" s="108"/>
-      <c r="AI3" s="108"/>
-      <c r="AJ3" s="108"/>
-      <c r="AK3" s="108"/>
-      <c r="AL3" s="108"/>
-      <c r="AM3" s="108"/>
-      <c r="AN3" s="108"/>
-      <c r="AO3" s="108"/>
-      <c r="AP3" s="108"/>
-      <c r="AQ3" s="108"/>
-      <c r="AR3" s="108"/>
-      <c r="AS3" s="108"/>
-      <c r="AT3" s="108"/>
-      <c r="AU3" s="108"/>
-      <c r="AV3" s="108"/>
-      <c r="AW3" s="108"/>
-      <c r="AX3" s="108"/>
-      <c r="AY3" s="108"/>
-      <c r="AZ3" s="108"/>
-      <c r="BA3" s="108"/>
-      <c r="BB3" s="108"/>
-      <c r="BC3" s="108"/>
-      <c r="BD3" s="108"/>
-      <c r="BE3" s="108"/>
-      <c r="BF3" s="108"/>
-      <c r="BG3" s="108"/>
-      <c r="BH3" s="108"/>
-      <c r="BI3" s="108"/>
-      <c r="BJ3" s="108"/>
-      <c r="BK3" s="108"/>
-      <c r="BL3" s="108"/>
-      <c r="BM3" s="108"/>
-      <c r="BN3" s="108"/>
-      <c r="BO3" s="108"/>
-      <c r="BP3" s="108"/>
-      <c r="BQ3" s="108"/>
-      <c r="BR3" s="108"/>
-      <c r="BS3" s="108"/>
-      <c r="BT3" s="108"/>
-      <c r="BU3" s="108"/>
-      <c r="BV3" s="108"/>
-      <c r="BW3" s="108"/>
-      <c r="BX3" s="108"/>
-      <c r="BY3" s="108"/>
-      <c r="BZ3" s="108"/>
-      <c r="CA3" s="108"/>
-      <c r="CB3" s="108"/>
-      <c r="CC3" s="108"/>
-      <c r="CD3" s="108"/>
-      <c r="CE3" s="108"/>
-      <c r="CF3" s="108"/>
-      <c r="CG3" s="108"/>
-      <c r="CH3" s="108"/>
-      <c r="CI3" s="108"/>
-      <c r="CJ3" s="108"/>
-      <c r="CK3" s="108"/>
-      <c r="CL3" s="108"/>
-      <c r="CM3" s="108"/>
-      <c r="CN3" s="108"/>
-      <c r="CO3" s="108"/>
-      <c r="CP3" s="108"/>
-      <c r="CQ3" s="108"/>
-      <c r="CR3" s="108"/>
-      <c r="CS3" s="108"/>
-      <c r="CT3" s="108"/>
-      <c r="CU3" s="108"/>
-      <c r="CV3" s="108"/>
-      <c r="CW3" s="108"/>
-      <c r="CX3" s="108"/>
-      <c r="CY3" s="108"/>
-      <c r="CZ3" s="108"/>
-      <c r="DA3" s="108"/>
-      <c r="DB3" s="108"/>
-      <c r="DC3" s="108"/>
-      <c r="DD3" s="108"/>
-      <c r="DE3" s="108"/>
-      <c r="DF3" s="108"/>
-      <c r="DG3" s="108"/>
-      <c r="DH3" s="108"/>
-      <c r="DI3" s="108"/>
-      <c r="DJ3" s="108"/>
-      <c r="DK3" s="108"/>
-      <c r="DL3" s="108"/>
-      <c r="DM3" s="108"/>
-      <c r="DN3" s="108"/>
-      <c r="DO3" s="108"/>
-      <c r="DP3" s="108"/>
-      <c r="DQ3" s="108"/>
-      <c r="DR3" s="108"/>
-      <c r="DS3" s="108"/>
-      <c r="DT3" s="108"/>
-      <c r="DU3" s="108"/>
-      <c r="DV3" s="108"/>
-      <c r="DW3" s="108"/>
-      <c r="DX3" s="108"/>
-      <c r="DY3" s="108"/>
-      <c r="DZ3" s="108"/>
-      <c r="EA3" s="108"/>
-      <c r="EB3" s="108"/>
-      <c r="EC3" s="108"/>
-      <c r="ED3" s="108"/>
-      <c r="EE3" s="108"/>
-      <c r="EF3" s="108"/>
-      <c r="EG3" s="108"/>
-      <c r="EH3" s="108"/>
-      <c r="EI3" s="108"/>
-      <c r="EJ3" s="108"/>
-      <c r="EK3" s="108"/>
-      <c r="EL3" s="108"/>
-      <c r="EM3" s="108"/>
-      <c r="EN3" s="108"/>
-      <c r="EO3" s="108"/>
-      <c r="EP3" s="108"/>
-      <c r="EQ3" s="108"/>
-      <c r="ER3" s="108"/>
-      <c r="ES3" s="108"/>
-      <c r="ET3" s="108"/>
-      <c r="EU3" s="108"/>
-      <c r="EV3" s="108"/>
-      <c r="EW3" s="108"/>
-      <c r="EX3" s="108"/>
-      <c r="EY3" s="108"/>
-      <c r="EZ3" s="108"/>
-      <c r="FA3" s="108"/>
-      <c r="FB3" s="108"/>
-      <c r="FC3" s="108"/>
-      <c r="FD3" s="108"/>
-      <c r="FE3" s="108"/>
-      <c r="FF3" s="108"/>
-      <c r="FG3" s="108"/>
-      <c r="FH3" s="108"/>
-      <c r="FI3" s="108"/>
-      <c r="FJ3" s="108"/>
-      <c r="FK3" s="108"/>
-      <c r="FL3" s="108"/>
-      <c r="FM3" s="108"/>
-      <c r="FN3" s="108"/>
-      <c r="FO3" s="108"/>
-      <c r="FP3" s="108"/>
-      <c r="FQ3" s="108"/>
-      <c r="FR3" s="108"/>
-      <c r="FS3" s="108"/>
-      <c r="FT3" s="108"/>
-      <c r="FU3" s="108"/>
-      <c r="FV3" s="108"/>
-      <c r="FW3" s="108"/>
-      <c r="FX3" s="108"/>
-      <c r="FY3" s="108"/>
-      <c r="FZ3" s="108"/>
-      <c r="GA3" s="108"/>
-      <c r="GB3" s="108"/>
-      <c r="GC3" s="108"/>
-      <c r="GD3" s="108"/>
-      <c r="GE3" s="108"/>
-      <c r="GF3" s="108"/>
-      <c r="GG3" s="108"/>
-      <c r="GH3" s="108"/>
-      <c r="GI3" s="108"/>
-      <c r="GJ3" s="108"/>
-      <c r="GK3" s="108"/>
-      <c r="GL3" s="108"/>
-      <c r="GM3" s="108"/>
-      <c r="GN3" s="108"/>
-      <c r="GO3" s="108"/>
-      <c r="GP3" s="108"/>
-      <c r="GQ3" s="108"/>
-      <c r="GR3" s="108"/>
-      <c r="GS3" s="108"/>
-      <c r="GT3" s="108"/>
-      <c r="GU3" s="108"/>
-      <c r="GV3" s="108"/>
-      <c r="GW3" s="108"/>
-      <c r="GX3" s="108"/>
-      <c r="GY3" s="108"/>
-      <c r="GZ3" s="108"/>
-      <c r="HA3" s="108"/>
-      <c r="HB3" s="108"/>
-      <c r="HC3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
+      <c r="AB3" s="109"/>
+      <c r="AC3" s="109"/>
+      <c r="AD3" s="109"/>
+      <c r="AE3" s="109"/>
+      <c r="AF3" s="109"/>
+      <c r="AG3" s="109"/>
+      <c r="AH3" s="109"/>
+      <c r="AI3" s="109"/>
+      <c r="AJ3" s="109"/>
+      <c r="AK3" s="109"/>
+      <c r="AL3" s="109"/>
+      <c r="AM3" s="109"/>
+      <c r="AN3" s="109"/>
+      <c r="AO3" s="109"/>
+      <c r="AP3" s="109"/>
+      <c r="AQ3" s="109"/>
+      <c r="AR3" s="109"/>
+      <c r="AS3" s="109"/>
+      <c r="AT3" s="109"/>
+      <c r="AU3" s="109"/>
+      <c r="AV3" s="109"/>
+      <c r="AW3" s="109"/>
+      <c r="AX3" s="109"/>
+      <c r="AY3" s="109"/>
+      <c r="AZ3" s="109"/>
+      <c r="BA3" s="109"/>
+      <c r="BB3" s="109"/>
+      <c r="BC3" s="109"/>
+      <c r="BD3" s="109"/>
+      <c r="BE3" s="109"/>
+      <c r="BF3" s="109"/>
+      <c r="BG3" s="109"/>
+      <c r="BH3" s="109"/>
+      <c r="BI3" s="109"/>
+      <c r="BJ3" s="109"/>
+      <c r="BK3" s="109"/>
+      <c r="BL3" s="109"/>
+      <c r="BM3" s="109"/>
+      <c r="BN3" s="109"/>
+      <c r="BO3" s="109"/>
+      <c r="BP3" s="109"/>
+      <c r="BQ3" s="109"/>
+      <c r="BR3" s="109"/>
+      <c r="BS3" s="109"/>
+      <c r="BT3" s="109"/>
+      <c r="BU3" s="109"/>
+      <c r="BV3" s="109"/>
+      <c r="BW3" s="109"/>
+      <c r="BX3" s="109"/>
+      <c r="BY3" s="109"/>
+      <c r="BZ3" s="109"/>
+      <c r="CA3" s="109"/>
+      <c r="CB3" s="109"/>
+      <c r="CC3" s="109"/>
+      <c r="CD3" s="109"/>
+      <c r="CE3" s="109"/>
+      <c r="CF3" s="109"/>
+      <c r="CG3" s="109"/>
+      <c r="CH3" s="109"/>
+      <c r="CI3" s="109"/>
+      <c r="CJ3" s="109"/>
+      <c r="CK3" s="109"/>
+      <c r="CL3" s="109"/>
+      <c r="CM3" s="109"/>
+      <c r="CN3" s="109"/>
+      <c r="CO3" s="109"/>
+      <c r="CP3" s="109"/>
+      <c r="CQ3" s="109"/>
+      <c r="CR3" s="109"/>
+      <c r="CS3" s="109"/>
+      <c r="CT3" s="109"/>
+      <c r="CU3" s="109"/>
+      <c r="CV3" s="109"/>
+      <c r="CW3" s="109"/>
+      <c r="CX3" s="109"/>
+      <c r="CY3" s="109"/>
+      <c r="CZ3" s="109"/>
+      <c r="DA3" s="109"/>
+      <c r="DB3" s="109"/>
+      <c r="DC3" s="109"/>
+      <c r="DD3" s="109"/>
+      <c r="DE3" s="109"/>
+      <c r="DF3" s="109"/>
+      <c r="DG3" s="109"/>
+      <c r="DH3" s="109"/>
+      <c r="DI3" s="109"/>
+      <c r="DJ3" s="109"/>
+      <c r="DK3" s="109"/>
+      <c r="DL3" s="109"/>
+      <c r="DM3" s="109"/>
+      <c r="DN3" s="109"/>
+      <c r="DO3" s="109"/>
+      <c r="DP3" s="109"/>
+      <c r="DQ3" s="109"/>
+      <c r="DR3" s="109"/>
+      <c r="DS3" s="109"/>
+      <c r="DT3" s="109"/>
+      <c r="DU3" s="109"/>
+      <c r="DV3" s="109"/>
+      <c r="DW3" s="109"/>
+      <c r="DX3" s="109"/>
+      <c r="DY3" s="109"/>
+      <c r="DZ3" s="109"/>
+      <c r="EA3" s="109"/>
+      <c r="EB3" s="109"/>
+      <c r="EC3" s="109"/>
+      <c r="ED3" s="109"/>
+      <c r="EE3" s="109"/>
+      <c r="EF3" s="109"/>
+      <c r="EG3" s="109"/>
+      <c r="EH3" s="109"/>
+      <c r="EI3" s="109"/>
+      <c r="EJ3" s="109"/>
+      <c r="EK3" s="109"/>
+      <c r="EL3" s="109"/>
+      <c r="EM3" s="109"/>
+      <c r="EN3" s="109"/>
+      <c r="EO3" s="109"/>
+      <c r="EP3" s="109"/>
+      <c r="EQ3" s="109"/>
+      <c r="ER3" s="109"/>
+      <c r="ES3" s="109"/>
+      <c r="ET3" s="109"/>
+      <c r="EU3" s="109"/>
+      <c r="EV3" s="109"/>
+      <c r="EW3" s="109"/>
+      <c r="EX3" s="109"/>
+      <c r="EY3" s="109"/>
+      <c r="EZ3" s="109"/>
+      <c r="FA3" s="109"/>
+      <c r="FB3" s="109"/>
+      <c r="FC3" s="109"/>
+      <c r="FD3" s="109"/>
+      <c r="FE3" s="109"/>
+      <c r="FF3" s="109"/>
+      <c r="FG3" s="109"/>
+      <c r="FH3" s="109"/>
+      <c r="FI3" s="109"/>
+      <c r="FJ3" s="109"/>
+      <c r="FK3" s="109"/>
+      <c r="FL3" s="109"/>
+      <c r="FM3" s="109"/>
+      <c r="FN3" s="109"/>
+      <c r="FO3" s="109"/>
+      <c r="FP3" s="109"/>
+      <c r="FQ3" s="109"/>
+      <c r="FR3" s="109"/>
+      <c r="FS3" s="109"/>
+      <c r="FT3" s="109"/>
+      <c r="FU3" s="109"/>
+      <c r="FV3" s="109"/>
+      <c r="FW3" s="109"/>
+      <c r="FX3" s="109"/>
+      <c r="FY3" s="109"/>
+      <c r="FZ3" s="109"/>
+      <c r="GA3" s="109"/>
+      <c r="GB3" s="109"/>
+      <c r="GC3" s="109"/>
+      <c r="GD3" s="109"/>
+      <c r="GE3" s="109"/>
+      <c r="GF3" s="109"/>
+      <c r="GG3" s="109"/>
+      <c r="GH3" s="109"/>
+      <c r="GI3" s="109"/>
+      <c r="GJ3" s="109"/>
+      <c r="GK3" s="109"/>
+      <c r="GL3" s="109"/>
+      <c r="GM3" s="109"/>
+      <c r="GN3" s="109"/>
+      <c r="GO3" s="109"/>
+      <c r="GP3" s="109"/>
+      <c r="GQ3" s="109"/>
+      <c r="GR3" s="109"/>
+      <c r="GS3" s="109"/>
+      <c r="GT3" s="109"/>
+      <c r="GU3" s="109"/>
+      <c r="GV3" s="109"/>
+      <c r="GW3" s="109"/>
+      <c r="GX3" s="109"/>
+      <c r="GY3" s="109"/>
+      <c r="GZ3" s="109"/>
+      <c r="HA3" s="109"/>
+      <c r="HB3" s="109"/>
+      <c r="HC3" s="110"/>
     </row>
     <row r="4" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="89" t="s">
-        <v>21</v>
+      <c r="B4" s="90" t="s">
+        <v>34</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="99"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="98" t="s">
+      <c r="G4" s="100"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="101"/>
       <c r="K4" s="61" t="s">
         <v>12</v>
       </c>
@@ -2460,15 +2460,15 @@
       <c r="HC4" s="28"/>
     </row>
     <row r="5" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="92"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="103"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="104"/>
       <c r="K5" s="51" t="s">
         <v>11</v>
       </c>
@@ -2674,15 +2674,15 @@
       <c r="HC5" s="28"/>
     </row>
     <row r="6" spans="1:211" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="95"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="106"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="107"/>
       <c r="K6" s="51" t="s">
         <v>19</v>
       </c>
@@ -2895,12 +2895,12 @@
         <v>5</v>
       </c>
       <c r="D7" s="55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="F7" s="112" t="s">
+      <c r="F7" s="79" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="57" t="s">
@@ -2916,7 +2916,7 @@
         <v>20</v>
       </c>
       <c r="K7" s="62" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L7" s="29"/>
       <c r="M7" s="30"/>
@@ -4073,7 +4073,7 @@
       <c r="HC1048575" s="47"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GZrKIrqnpAc6NX5OZ2neCpMXMDVf/SA7eF5KW7FXmzSsOAKoMj+t2oDjDjVL2ryevIUDA+H1TPHIrcz4oWzhFg==" saltValue="vkusKh8xY+iml5BT24wx8Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7y30xUDt19rWnUkEQecomBB6U3TesPo1zIQt5KuetdcxPNveuCy0au6mtZqQUzv9gQBEfL6GPDrN1yO8U17XeA==" saltValue="PQ1Y3bVNWcuOHWop+u1utg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B4:E6"/>
     <mergeCell ref="F4:H6"/>

</xml_diff>

<commit_message>
Edits in forms descriptions and conversion of dates in XLSX forms
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1DI.xlsx
+++ b/form_reporting_templates/Form-1DI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\Data dissemination\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379A498E-36BB-481D-93EC-DC2A5A54638A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6468A58C-C8D8-427A-A2B5-EBF610DA836F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -174,8 +174,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -884,10 +884,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1140,6 +1136,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1175,9 +1175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1215,7 +1215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1321,7 +1321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1463,7 +1463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1489,24 +1489,24 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="86"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="87"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="89"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="88"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1556,15 +1556,15 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="82"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="83"/>
+      <c r="G8" s="82"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1607,7 +1607,7 @@
       <c r="C12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="112"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1618,7 +1618,7 @@
       <c r="C13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="112"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1667,7 +1667,7 @@
       <c r="C18" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="39"/>
       <c r="E18" s="10"/>
       <c r="F18" s="14"/>
       <c r="G18" s="23"/>
@@ -1675,10 +1675,10 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="39"/>
       <c r="E19" s="10"/>
       <c r="F19" s="14"/>
       <c r="G19" s="17"/>
@@ -1686,10 +1686,10 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="D20" s="39"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -1735,11 +1735,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="82"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="81"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1756,7 +1756,7 @@
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2UXIQAtCAe1Hl3LOIP95j6T5lN4CreFbp/G7xZfYEjLnpx98jtQhpQhWmp07FYOVM1xMp78hncUia1FB6wrMWw==" saltValue="HvcaMeX3WSxt5je20kTU3g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qzzWBlZZUVBt3RoNQOKuUOqB4TFmwsWjMhr2d3TjT7WEcJJt/O6k8cSlBfdipxgawf2q30/RSpWug0+BawY5pw==" saltValue="8HpRcGRg8db+djtBnAW3fw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>
@@ -1791,19 +1791,19 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="63" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="64" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="64" customWidth="1"/>
-    <col min="5" max="5" width="14" style="65" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="63" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="64" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="66" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="63" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="69" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" style="77" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="73"/>
-    <col min="13" max="210" width="9.140625" style="74"/>
-    <col min="211" max="211" width="9.140625" style="75"/>
+    <col min="2" max="2" width="11.42578125" style="62" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="63" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="63" customWidth="1"/>
+    <col min="5" max="5" width="14" style="64" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="62" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="63" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="65" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="62" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="68" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" style="76" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="72"/>
+    <col min="13" max="210" width="9.140625" style="73"/>
+    <col min="211" max="211" width="9.140625" style="74"/>
     <col min="212" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
@@ -1811,18 +1811,18 @@
       <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="111"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="110"/>
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
@@ -2026,236 +2026,236 @@
     </row>
     <row r="3" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
-      <c r="B3" s="87"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="108" t="s">
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="111"/>
+      <c r="L3" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="109"/>
-      <c r="N3" s="109"/>
-      <c r="O3" s="109"/>
-      <c r="P3" s="109"/>
-      <c r="Q3" s="109"/>
-      <c r="R3" s="109"/>
-      <c r="S3" s="109"/>
-      <c r="T3" s="109"/>
-      <c r="U3" s="109"/>
-      <c r="V3" s="109"/>
-      <c r="W3" s="109"/>
-      <c r="X3" s="109"/>
-      <c r="Y3" s="109"/>
-      <c r="Z3" s="109"/>
-      <c r="AA3" s="109"/>
-      <c r="AB3" s="109"/>
-      <c r="AC3" s="109"/>
-      <c r="AD3" s="109"/>
-      <c r="AE3" s="109"/>
-      <c r="AF3" s="109"/>
-      <c r="AG3" s="109"/>
-      <c r="AH3" s="109"/>
-      <c r="AI3" s="109"/>
-      <c r="AJ3" s="109"/>
-      <c r="AK3" s="109"/>
-      <c r="AL3" s="109"/>
-      <c r="AM3" s="109"/>
-      <c r="AN3" s="109"/>
-      <c r="AO3" s="109"/>
-      <c r="AP3" s="109"/>
-      <c r="AQ3" s="109"/>
-      <c r="AR3" s="109"/>
-      <c r="AS3" s="109"/>
-      <c r="AT3" s="109"/>
-      <c r="AU3" s="109"/>
-      <c r="AV3" s="109"/>
-      <c r="AW3" s="109"/>
-      <c r="AX3" s="109"/>
-      <c r="AY3" s="109"/>
-      <c r="AZ3" s="109"/>
-      <c r="BA3" s="109"/>
-      <c r="BB3" s="109"/>
-      <c r="BC3" s="109"/>
-      <c r="BD3" s="109"/>
-      <c r="BE3" s="109"/>
-      <c r="BF3" s="109"/>
-      <c r="BG3" s="109"/>
-      <c r="BH3" s="109"/>
-      <c r="BI3" s="109"/>
-      <c r="BJ3" s="109"/>
-      <c r="BK3" s="109"/>
-      <c r="BL3" s="109"/>
-      <c r="BM3" s="109"/>
-      <c r="BN3" s="109"/>
-      <c r="BO3" s="109"/>
-      <c r="BP3" s="109"/>
-      <c r="BQ3" s="109"/>
-      <c r="BR3" s="109"/>
-      <c r="BS3" s="109"/>
-      <c r="BT3" s="109"/>
-      <c r="BU3" s="109"/>
-      <c r="BV3" s="109"/>
-      <c r="BW3" s="109"/>
-      <c r="BX3" s="109"/>
-      <c r="BY3" s="109"/>
-      <c r="BZ3" s="109"/>
-      <c r="CA3" s="109"/>
-      <c r="CB3" s="109"/>
-      <c r="CC3" s="109"/>
-      <c r="CD3" s="109"/>
-      <c r="CE3" s="109"/>
-      <c r="CF3" s="109"/>
-      <c r="CG3" s="109"/>
-      <c r="CH3" s="109"/>
-      <c r="CI3" s="109"/>
-      <c r="CJ3" s="109"/>
-      <c r="CK3" s="109"/>
-      <c r="CL3" s="109"/>
-      <c r="CM3" s="109"/>
-      <c r="CN3" s="109"/>
-      <c r="CO3" s="109"/>
-      <c r="CP3" s="109"/>
-      <c r="CQ3" s="109"/>
-      <c r="CR3" s="109"/>
-      <c r="CS3" s="109"/>
-      <c r="CT3" s="109"/>
-      <c r="CU3" s="109"/>
-      <c r="CV3" s="109"/>
-      <c r="CW3" s="109"/>
-      <c r="CX3" s="109"/>
-      <c r="CY3" s="109"/>
-      <c r="CZ3" s="109"/>
-      <c r="DA3" s="109"/>
-      <c r="DB3" s="109"/>
-      <c r="DC3" s="109"/>
-      <c r="DD3" s="109"/>
-      <c r="DE3" s="109"/>
-      <c r="DF3" s="109"/>
-      <c r="DG3" s="109"/>
-      <c r="DH3" s="109"/>
-      <c r="DI3" s="109"/>
-      <c r="DJ3" s="109"/>
-      <c r="DK3" s="109"/>
-      <c r="DL3" s="109"/>
-      <c r="DM3" s="109"/>
-      <c r="DN3" s="109"/>
-      <c r="DO3" s="109"/>
-      <c r="DP3" s="109"/>
-      <c r="DQ3" s="109"/>
-      <c r="DR3" s="109"/>
-      <c r="DS3" s="109"/>
-      <c r="DT3" s="109"/>
-      <c r="DU3" s="109"/>
-      <c r="DV3" s="109"/>
-      <c r="DW3" s="109"/>
-      <c r="DX3" s="109"/>
-      <c r="DY3" s="109"/>
-      <c r="DZ3" s="109"/>
-      <c r="EA3" s="109"/>
-      <c r="EB3" s="109"/>
-      <c r="EC3" s="109"/>
-      <c r="ED3" s="109"/>
-      <c r="EE3" s="109"/>
-      <c r="EF3" s="109"/>
-      <c r="EG3" s="109"/>
-      <c r="EH3" s="109"/>
-      <c r="EI3" s="109"/>
-      <c r="EJ3" s="109"/>
-      <c r="EK3" s="109"/>
-      <c r="EL3" s="109"/>
-      <c r="EM3" s="109"/>
-      <c r="EN3" s="109"/>
-      <c r="EO3" s="109"/>
-      <c r="EP3" s="109"/>
-      <c r="EQ3" s="109"/>
-      <c r="ER3" s="109"/>
-      <c r="ES3" s="109"/>
-      <c r="ET3" s="109"/>
-      <c r="EU3" s="109"/>
-      <c r="EV3" s="109"/>
-      <c r="EW3" s="109"/>
-      <c r="EX3" s="109"/>
-      <c r="EY3" s="109"/>
-      <c r="EZ3" s="109"/>
-      <c r="FA3" s="109"/>
-      <c r="FB3" s="109"/>
-      <c r="FC3" s="109"/>
-      <c r="FD3" s="109"/>
-      <c r="FE3" s="109"/>
-      <c r="FF3" s="109"/>
-      <c r="FG3" s="109"/>
-      <c r="FH3" s="109"/>
-      <c r="FI3" s="109"/>
-      <c r="FJ3" s="109"/>
-      <c r="FK3" s="109"/>
-      <c r="FL3" s="109"/>
-      <c r="FM3" s="109"/>
-      <c r="FN3" s="109"/>
-      <c r="FO3" s="109"/>
-      <c r="FP3" s="109"/>
-      <c r="FQ3" s="109"/>
-      <c r="FR3" s="109"/>
-      <c r="FS3" s="109"/>
-      <c r="FT3" s="109"/>
-      <c r="FU3" s="109"/>
-      <c r="FV3" s="109"/>
-      <c r="FW3" s="109"/>
-      <c r="FX3" s="109"/>
-      <c r="FY3" s="109"/>
-      <c r="FZ3" s="109"/>
-      <c r="GA3" s="109"/>
-      <c r="GB3" s="109"/>
-      <c r="GC3" s="109"/>
-      <c r="GD3" s="109"/>
-      <c r="GE3" s="109"/>
-      <c r="GF3" s="109"/>
-      <c r="GG3" s="109"/>
-      <c r="GH3" s="109"/>
-      <c r="GI3" s="109"/>
-      <c r="GJ3" s="109"/>
-      <c r="GK3" s="109"/>
-      <c r="GL3" s="109"/>
-      <c r="GM3" s="109"/>
-      <c r="GN3" s="109"/>
-      <c r="GO3" s="109"/>
-      <c r="GP3" s="109"/>
-      <c r="GQ3" s="109"/>
-      <c r="GR3" s="109"/>
-      <c r="GS3" s="109"/>
-      <c r="GT3" s="109"/>
-      <c r="GU3" s="109"/>
-      <c r="GV3" s="109"/>
-      <c r="GW3" s="109"/>
-      <c r="GX3" s="109"/>
-      <c r="GY3" s="109"/>
-      <c r="GZ3" s="109"/>
-      <c r="HA3" s="109"/>
-      <c r="HB3" s="109"/>
-      <c r="HC3" s="110"/>
+      <c r="M3" s="108"/>
+      <c r="N3" s="108"/>
+      <c r="O3" s="108"/>
+      <c r="P3" s="108"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="108"/>
+      <c r="S3" s="108"/>
+      <c r="T3" s="108"/>
+      <c r="U3" s="108"/>
+      <c r="V3" s="108"/>
+      <c r="W3" s="108"/>
+      <c r="X3" s="108"/>
+      <c r="Y3" s="108"/>
+      <c r="Z3" s="108"/>
+      <c r="AA3" s="108"/>
+      <c r="AB3" s="108"/>
+      <c r="AC3" s="108"/>
+      <c r="AD3" s="108"/>
+      <c r="AE3" s="108"/>
+      <c r="AF3" s="108"/>
+      <c r="AG3" s="108"/>
+      <c r="AH3" s="108"/>
+      <c r="AI3" s="108"/>
+      <c r="AJ3" s="108"/>
+      <c r="AK3" s="108"/>
+      <c r="AL3" s="108"/>
+      <c r="AM3" s="108"/>
+      <c r="AN3" s="108"/>
+      <c r="AO3" s="108"/>
+      <c r="AP3" s="108"/>
+      <c r="AQ3" s="108"/>
+      <c r="AR3" s="108"/>
+      <c r="AS3" s="108"/>
+      <c r="AT3" s="108"/>
+      <c r="AU3" s="108"/>
+      <c r="AV3" s="108"/>
+      <c r="AW3" s="108"/>
+      <c r="AX3" s="108"/>
+      <c r="AY3" s="108"/>
+      <c r="AZ3" s="108"/>
+      <c r="BA3" s="108"/>
+      <c r="BB3" s="108"/>
+      <c r="BC3" s="108"/>
+      <c r="BD3" s="108"/>
+      <c r="BE3" s="108"/>
+      <c r="BF3" s="108"/>
+      <c r="BG3" s="108"/>
+      <c r="BH3" s="108"/>
+      <c r="BI3" s="108"/>
+      <c r="BJ3" s="108"/>
+      <c r="BK3" s="108"/>
+      <c r="BL3" s="108"/>
+      <c r="BM3" s="108"/>
+      <c r="BN3" s="108"/>
+      <c r="BO3" s="108"/>
+      <c r="BP3" s="108"/>
+      <c r="BQ3" s="108"/>
+      <c r="BR3" s="108"/>
+      <c r="BS3" s="108"/>
+      <c r="BT3" s="108"/>
+      <c r="BU3" s="108"/>
+      <c r="BV3" s="108"/>
+      <c r="BW3" s="108"/>
+      <c r="BX3" s="108"/>
+      <c r="BY3" s="108"/>
+      <c r="BZ3" s="108"/>
+      <c r="CA3" s="108"/>
+      <c r="CB3" s="108"/>
+      <c r="CC3" s="108"/>
+      <c r="CD3" s="108"/>
+      <c r="CE3" s="108"/>
+      <c r="CF3" s="108"/>
+      <c r="CG3" s="108"/>
+      <c r="CH3" s="108"/>
+      <c r="CI3" s="108"/>
+      <c r="CJ3" s="108"/>
+      <c r="CK3" s="108"/>
+      <c r="CL3" s="108"/>
+      <c r="CM3" s="108"/>
+      <c r="CN3" s="108"/>
+      <c r="CO3" s="108"/>
+      <c r="CP3" s="108"/>
+      <c r="CQ3" s="108"/>
+      <c r="CR3" s="108"/>
+      <c r="CS3" s="108"/>
+      <c r="CT3" s="108"/>
+      <c r="CU3" s="108"/>
+      <c r="CV3" s="108"/>
+      <c r="CW3" s="108"/>
+      <c r="CX3" s="108"/>
+      <c r="CY3" s="108"/>
+      <c r="CZ3" s="108"/>
+      <c r="DA3" s="108"/>
+      <c r="DB3" s="108"/>
+      <c r="DC3" s="108"/>
+      <c r="DD3" s="108"/>
+      <c r="DE3" s="108"/>
+      <c r="DF3" s="108"/>
+      <c r="DG3" s="108"/>
+      <c r="DH3" s="108"/>
+      <c r="DI3" s="108"/>
+      <c r="DJ3" s="108"/>
+      <c r="DK3" s="108"/>
+      <c r="DL3" s="108"/>
+      <c r="DM3" s="108"/>
+      <c r="DN3" s="108"/>
+      <c r="DO3" s="108"/>
+      <c r="DP3" s="108"/>
+      <c r="DQ3" s="108"/>
+      <c r="DR3" s="108"/>
+      <c r="DS3" s="108"/>
+      <c r="DT3" s="108"/>
+      <c r="DU3" s="108"/>
+      <c r="DV3" s="108"/>
+      <c r="DW3" s="108"/>
+      <c r="DX3" s="108"/>
+      <c r="DY3" s="108"/>
+      <c r="DZ3" s="108"/>
+      <c r="EA3" s="108"/>
+      <c r="EB3" s="108"/>
+      <c r="EC3" s="108"/>
+      <c r="ED3" s="108"/>
+      <c r="EE3" s="108"/>
+      <c r="EF3" s="108"/>
+      <c r="EG3" s="108"/>
+      <c r="EH3" s="108"/>
+      <c r="EI3" s="108"/>
+      <c r="EJ3" s="108"/>
+      <c r="EK3" s="108"/>
+      <c r="EL3" s="108"/>
+      <c r="EM3" s="108"/>
+      <c r="EN3" s="108"/>
+      <c r="EO3" s="108"/>
+      <c r="EP3" s="108"/>
+      <c r="EQ3" s="108"/>
+      <c r="ER3" s="108"/>
+      <c r="ES3" s="108"/>
+      <c r="ET3" s="108"/>
+      <c r="EU3" s="108"/>
+      <c r="EV3" s="108"/>
+      <c r="EW3" s="108"/>
+      <c r="EX3" s="108"/>
+      <c r="EY3" s="108"/>
+      <c r="EZ3" s="108"/>
+      <c r="FA3" s="108"/>
+      <c r="FB3" s="108"/>
+      <c r="FC3" s="108"/>
+      <c r="FD3" s="108"/>
+      <c r="FE3" s="108"/>
+      <c r="FF3" s="108"/>
+      <c r="FG3" s="108"/>
+      <c r="FH3" s="108"/>
+      <c r="FI3" s="108"/>
+      <c r="FJ3" s="108"/>
+      <c r="FK3" s="108"/>
+      <c r="FL3" s="108"/>
+      <c r="FM3" s="108"/>
+      <c r="FN3" s="108"/>
+      <c r="FO3" s="108"/>
+      <c r="FP3" s="108"/>
+      <c r="FQ3" s="108"/>
+      <c r="FR3" s="108"/>
+      <c r="FS3" s="108"/>
+      <c r="FT3" s="108"/>
+      <c r="FU3" s="108"/>
+      <c r="FV3" s="108"/>
+      <c r="FW3" s="108"/>
+      <c r="FX3" s="108"/>
+      <c r="FY3" s="108"/>
+      <c r="FZ3" s="108"/>
+      <c r="GA3" s="108"/>
+      <c r="GB3" s="108"/>
+      <c r="GC3" s="108"/>
+      <c r="GD3" s="108"/>
+      <c r="GE3" s="108"/>
+      <c r="GF3" s="108"/>
+      <c r="GG3" s="108"/>
+      <c r="GH3" s="108"/>
+      <c r="GI3" s="108"/>
+      <c r="GJ3" s="108"/>
+      <c r="GK3" s="108"/>
+      <c r="GL3" s="108"/>
+      <c r="GM3" s="108"/>
+      <c r="GN3" s="108"/>
+      <c r="GO3" s="108"/>
+      <c r="GP3" s="108"/>
+      <c r="GQ3" s="108"/>
+      <c r="GR3" s="108"/>
+      <c r="GS3" s="108"/>
+      <c r="GT3" s="108"/>
+      <c r="GU3" s="108"/>
+      <c r="GV3" s="108"/>
+      <c r="GW3" s="108"/>
+      <c r="GX3" s="108"/>
+      <c r="GY3" s="108"/>
+      <c r="GZ3" s="108"/>
+      <c r="HA3" s="108"/>
+      <c r="HB3" s="108"/>
+      <c r="HC3" s="109"/>
     </row>
     <row r="4" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="99" t="s">
+      <c r="C4" s="90"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="100"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="99" t="s">
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="101"/>
-      <c r="K4" s="61" t="s">
+      <c r="J4" s="100"/>
+      <c r="K4" s="60" t="s">
         <v>12</v>
       </c>
       <c r="L4" s="26"/>
@@ -2460,16 +2460,16 @@
       <c r="HC4" s="28"/>
     </row>
     <row r="5" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="93"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="103"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="51" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="103"/>
+      <c r="I5" s="101"/>
+      <c r="J5" s="103"/>
+      <c r="K5" s="50" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="26"/>
@@ -2674,16 +2674,16 @@
       <c r="HC5" s="28"/>
     </row>
     <row r="6" spans="1:211" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="96"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="51" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="104"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="50" t="s">
         <v>19</v>
       </c>
       <c r="L6" s="26"/>
@@ -2888,34 +2888,34 @@
       <c r="HC6" s="28"/>
     </row>
     <row r="7" spans="1:211" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="56" t="s">
+      <c r="E7" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="79" t="s">
+      <c r="F7" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="58" t="s">
+      <c r="H7" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="60" t="s">
+      <c r="J7" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="62" t="s">
+      <c r="K7" s="61" t="s">
         <v>24</v>
       </c>
       <c r="L7" s="29"/>
@@ -3120,957 +3120,957 @@
       <c r="HC7" s="31"/>
     </row>
     <row r="8" spans="1:211" x14ac:dyDescent="0.25">
-      <c r="B8" s="42"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
-      <c r="O8" s="71"/>
-      <c r="P8" s="71"/>
-      <c r="Q8" s="71"/>
-      <c r="R8" s="71"/>
-      <c r="S8" s="71"/>
-      <c r="T8" s="71"/>
-      <c r="U8" s="71"/>
-      <c r="V8" s="71"/>
-      <c r="W8" s="71"/>
-      <c r="X8" s="71"/>
-      <c r="Y8" s="71"/>
-      <c r="Z8" s="71"/>
-      <c r="AA8" s="71"/>
-      <c r="AB8" s="71"/>
-      <c r="AC8" s="71"/>
-      <c r="AD8" s="71"/>
-      <c r="AE8" s="71"/>
-      <c r="AF8" s="71"/>
-      <c r="AG8" s="71"/>
-      <c r="AH8" s="71"/>
-      <c r="AI8" s="71"/>
-      <c r="AJ8" s="71"/>
-      <c r="AK8" s="71"/>
-      <c r="AL8" s="71"/>
-      <c r="AM8" s="71"/>
-      <c r="AN8" s="71"/>
-      <c r="AO8" s="71"/>
-      <c r="AP8" s="71"/>
-      <c r="AQ8" s="71"/>
-      <c r="AR8" s="71"/>
-      <c r="AS8" s="71"/>
-      <c r="AT8" s="71"/>
-      <c r="AU8" s="71"/>
-      <c r="AV8" s="71"/>
-      <c r="AW8" s="71"/>
-      <c r="AX8" s="71"/>
-      <c r="AY8" s="71"/>
-      <c r="AZ8" s="71"/>
-      <c r="BA8" s="71"/>
-      <c r="BB8" s="71"/>
-      <c r="BC8" s="71"/>
-      <c r="BD8" s="71"/>
-      <c r="BE8" s="71"/>
-      <c r="BF8" s="71"/>
-      <c r="BG8" s="71"/>
-      <c r="BH8" s="71"/>
-      <c r="BI8" s="71"/>
-      <c r="BJ8" s="71"/>
-      <c r="BK8" s="71"/>
-      <c r="BL8" s="71"/>
-      <c r="BM8" s="71"/>
-      <c r="BN8" s="71"/>
-      <c r="BO8" s="71"/>
-      <c r="BP8" s="71"/>
-      <c r="BQ8" s="71"/>
-      <c r="BR8" s="71"/>
-      <c r="BS8" s="71"/>
-      <c r="BT8" s="71"/>
-      <c r="BU8" s="71"/>
-      <c r="BV8" s="71"/>
-      <c r="BW8" s="71"/>
-      <c r="BX8" s="71"/>
-      <c r="BY8" s="71"/>
-      <c r="BZ8" s="71"/>
-      <c r="CA8" s="71"/>
-      <c r="CB8" s="71"/>
-      <c r="CC8" s="71"/>
-      <c r="CD8" s="71"/>
-      <c r="CE8" s="71"/>
-      <c r="CF8" s="71"/>
-      <c r="CG8" s="71"/>
-      <c r="CH8" s="71"/>
-      <c r="CI8" s="71"/>
-      <c r="CJ8" s="71"/>
-      <c r="CK8" s="71"/>
-      <c r="CL8" s="71"/>
-      <c r="CM8" s="71"/>
-      <c r="CN8" s="71"/>
-      <c r="CO8" s="71"/>
-      <c r="CP8" s="71"/>
-      <c r="CQ8" s="71"/>
-      <c r="CR8" s="71"/>
-      <c r="CS8" s="71"/>
-      <c r="CT8" s="71"/>
-      <c r="CU8" s="71"/>
-      <c r="CV8" s="71"/>
-      <c r="CW8" s="71"/>
-      <c r="CX8" s="71"/>
-      <c r="CY8" s="71"/>
-      <c r="CZ8" s="71"/>
-      <c r="DA8" s="71"/>
-      <c r="DB8" s="71"/>
-      <c r="DC8" s="71"/>
-      <c r="DD8" s="71"/>
-      <c r="DE8" s="71"/>
-      <c r="DF8" s="71"/>
-      <c r="DG8" s="71"/>
-      <c r="DH8" s="71"/>
-      <c r="DI8" s="71"/>
-      <c r="DJ8" s="71"/>
-      <c r="DK8" s="71"/>
-      <c r="DL8" s="71"/>
-      <c r="DM8" s="71"/>
-      <c r="DN8" s="71"/>
-      <c r="DO8" s="71"/>
-      <c r="DP8" s="71"/>
-      <c r="DQ8" s="71"/>
-      <c r="DR8" s="71"/>
-      <c r="DS8" s="71"/>
-      <c r="DT8" s="71"/>
-      <c r="DU8" s="71"/>
-      <c r="DV8" s="71"/>
-      <c r="DW8" s="71"/>
-      <c r="DX8" s="71"/>
-      <c r="DY8" s="71"/>
-      <c r="DZ8" s="71"/>
-      <c r="EA8" s="71"/>
-      <c r="EB8" s="71"/>
-      <c r="EC8" s="71"/>
-      <c r="ED8" s="71"/>
-      <c r="EE8" s="71"/>
-      <c r="EF8" s="71"/>
-      <c r="EG8" s="71"/>
-      <c r="EH8" s="71"/>
-      <c r="EI8" s="71"/>
-      <c r="EJ8" s="71"/>
-      <c r="EK8" s="71"/>
-      <c r="EL8" s="71"/>
-      <c r="EM8" s="71"/>
-      <c r="EN8" s="71"/>
-      <c r="EO8" s="71"/>
-      <c r="EP8" s="71"/>
-      <c r="EQ8" s="71"/>
-      <c r="ER8" s="71"/>
-      <c r="ES8" s="71"/>
-      <c r="ET8" s="71"/>
-      <c r="EU8" s="71"/>
-      <c r="EV8" s="71"/>
-      <c r="EW8" s="71"/>
-      <c r="EX8" s="71"/>
-      <c r="EY8" s="71"/>
-      <c r="EZ8" s="71"/>
-      <c r="FA8" s="71"/>
-      <c r="FB8" s="71"/>
-      <c r="FC8" s="71"/>
-      <c r="FD8" s="71"/>
-      <c r="FE8" s="71"/>
-      <c r="FF8" s="71"/>
-      <c r="FG8" s="71"/>
-      <c r="FH8" s="71"/>
-      <c r="FI8" s="71"/>
-      <c r="FJ8" s="71"/>
-      <c r="FK8" s="71"/>
-      <c r="FL8" s="71"/>
-      <c r="FM8" s="71"/>
-      <c r="FN8" s="71"/>
-      <c r="FO8" s="71"/>
-      <c r="FP8" s="71"/>
-      <c r="FQ8" s="71"/>
-      <c r="FR8" s="71"/>
-      <c r="FS8" s="71"/>
-      <c r="FT8" s="71"/>
-      <c r="FU8" s="71"/>
-      <c r="FV8" s="71"/>
-      <c r="FW8" s="71"/>
-      <c r="FX8" s="71"/>
-      <c r="FY8" s="71"/>
-      <c r="FZ8" s="71"/>
-      <c r="GA8" s="71"/>
-      <c r="GB8" s="71"/>
-      <c r="GC8" s="71"/>
-      <c r="GD8" s="71"/>
-      <c r="GE8" s="71"/>
-      <c r="GF8" s="71"/>
-      <c r="GG8" s="71"/>
-      <c r="GH8" s="71"/>
-      <c r="GI8" s="71"/>
-      <c r="GJ8" s="71"/>
-      <c r="GK8" s="71"/>
-      <c r="GL8" s="71"/>
-      <c r="GM8" s="71"/>
-      <c r="GN8" s="71"/>
-      <c r="GO8" s="71"/>
-      <c r="GP8" s="71"/>
-      <c r="GQ8" s="71"/>
-      <c r="GR8" s="71"/>
-      <c r="GS8" s="71"/>
-      <c r="GT8" s="71"/>
-      <c r="GU8" s="71"/>
-      <c r="GV8" s="71"/>
-      <c r="GW8" s="71"/>
-      <c r="GX8" s="71"/>
-      <c r="GY8" s="71"/>
-      <c r="GZ8" s="71"/>
-      <c r="HA8" s="71"/>
-      <c r="HB8" s="71"/>
-      <c r="HC8" s="72"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
+      <c r="O8" s="70"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="70"/>
+      <c r="W8" s="70"/>
+      <c r="X8" s="70"/>
+      <c r="Y8" s="70"/>
+      <c r="Z8" s="70"/>
+      <c r="AA8" s="70"/>
+      <c r="AB8" s="70"/>
+      <c r="AC8" s="70"/>
+      <c r="AD8" s="70"/>
+      <c r="AE8" s="70"/>
+      <c r="AF8" s="70"/>
+      <c r="AG8" s="70"/>
+      <c r="AH8" s="70"/>
+      <c r="AI8" s="70"/>
+      <c r="AJ8" s="70"/>
+      <c r="AK8" s="70"/>
+      <c r="AL8" s="70"/>
+      <c r="AM8" s="70"/>
+      <c r="AN8" s="70"/>
+      <c r="AO8" s="70"/>
+      <c r="AP8" s="70"/>
+      <c r="AQ8" s="70"/>
+      <c r="AR8" s="70"/>
+      <c r="AS8" s="70"/>
+      <c r="AT8" s="70"/>
+      <c r="AU8" s="70"/>
+      <c r="AV8" s="70"/>
+      <c r="AW8" s="70"/>
+      <c r="AX8" s="70"/>
+      <c r="AY8" s="70"/>
+      <c r="AZ8" s="70"/>
+      <c r="BA8" s="70"/>
+      <c r="BB8" s="70"/>
+      <c r="BC8" s="70"/>
+      <c r="BD8" s="70"/>
+      <c r="BE8" s="70"/>
+      <c r="BF8" s="70"/>
+      <c r="BG8" s="70"/>
+      <c r="BH8" s="70"/>
+      <c r="BI8" s="70"/>
+      <c r="BJ8" s="70"/>
+      <c r="BK8" s="70"/>
+      <c r="BL8" s="70"/>
+      <c r="BM8" s="70"/>
+      <c r="BN8" s="70"/>
+      <c r="BO8" s="70"/>
+      <c r="BP8" s="70"/>
+      <c r="BQ8" s="70"/>
+      <c r="BR8" s="70"/>
+      <c r="BS8" s="70"/>
+      <c r="BT8" s="70"/>
+      <c r="BU8" s="70"/>
+      <c r="BV8" s="70"/>
+      <c r="BW8" s="70"/>
+      <c r="BX8" s="70"/>
+      <c r="BY8" s="70"/>
+      <c r="BZ8" s="70"/>
+      <c r="CA8" s="70"/>
+      <c r="CB8" s="70"/>
+      <c r="CC8" s="70"/>
+      <c r="CD8" s="70"/>
+      <c r="CE8" s="70"/>
+      <c r="CF8" s="70"/>
+      <c r="CG8" s="70"/>
+      <c r="CH8" s="70"/>
+      <c r="CI8" s="70"/>
+      <c r="CJ8" s="70"/>
+      <c r="CK8" s="70"/>
+      <c r="CL8" s="70"/>
+      <c r="CM8" s="70"/>
+      <c r="CN8" s="70"/>
+      <c r="CO8" s="70"/>
+      <c r="CP8" s="70"/>
+      <c r="CQ8" s="70"/>
+      <c r="CR8" s="70"/>
+      <c r="CS8" s="70"/>
+      <c r="CT8" s="70"/>
+      <c r="CU8" s="70"/>
+      <c r="CV8" s="70"/>
+      <c r="CW8" s="70"/>
+      <c r="CX8" s="70"/>
+      <c r="CY8" s="70"/>
+      <c r="CZ8" s="70"/>
+      <c r="DA8" s="70"/>
+      <c r="DB8" s="70"/>
+      <c r="DC8" s="70"/>
+      <c r="DD8" s="70"/>
+      <c r="DE8" s="70"/>
+      <c r="DF8" s="70"/>
+      <c r="DG8" s="70"/>
+      <c r="DH8" s="70"/>
+      <c r="DI8" s="70"/>
+      <c r="DJ8" s="70"/>
+      <c r="DK8" s="70"/>
+      <c r="DL8" s="70"/>
+      <c r="DM8" s="70"/>
+      <c r="DN8" s="70"/>
+      <c r="DO8" s="70"/>
+      <c r="DP8" s="70"/>
+      <c r="DQ8" s="70"/>
+      <c r="DR8" s="70"/>
+      <c r="DS8" s="70"/>
+      <c r="DT8" s="70"/>
+      <c r="DU8" s="70"/>
+      <c r="DV8" s="70"/>
+      <c r="DW8" s="70"/>
+      <c r="DX8" s="70"/>
+      <c r="DY8" s="70"/>
+      <c r="DZ8" s="70"/>
+      <c r="EA8" s="70"/>
+      <c r="EB8" s="70"/>
+      <c r="EC8" s="70"/>
+      <c r="ED8" s="70"/>
+      <c r="EE8" s="70"/>
+      <c r="EF8" s="70"/>
+      <c r="EG8" s="70"/>
+      <c r="EH8" s="70"/>
+      <c r="EI8" s="70"/>
+      <c r="EJ8" s="70"/>
+      <c r="EK8" s="70"/>
+      <c r="EL8" s="70"/>
+      <c r="EM8" s="70"/>
+      <c r="EN8" s="70"/>
+      <c r="EO8" s="70"/>
+      <c r="EP8" s="70"/>
+      <c r="EQ8" s="70"/>
+      <c r="ER8" s="70"/>
+      <c r="ES8" s="70"/>
+      <c r="ET8" s="70"/>
+      <c r="EU8" s="70"/>
+      <c r="EV8" s="70"/>
+      <c r="EW8" s="70"/>
+      <c r="EX8" s="70"/>
+      <c r="EY8" s="70"/>
+      <c r="EZ8" s="70"/>
+      <c r="FA8" s="70"/>
+      <c r="FB8" s="70"/>
+      <c r="FC8" s="70"/>
+      <c r="FD8" s="70"/>
+      <c r="FE8" s="70"/>
+      <c r="FF8" s="70"/>
+      <c r="FG8" s="70"/>
+      <c r="FH8" s="70"/>
+      <c r="FI8" s="70"/>
+      <c r="FJ8" s="70"/>
+      <c r="FK8" s="70"/>
+      <c r="FL8" s="70"/>
+      <c r="FM8" s="70"/>
+      <c r="FN8" s="70"/>
+      <c r="FO8" s="70"/>
+      <c r="FP8" s="70"/>
+      <c r="FQ8" s="70"/>
+      <c r="FR8" s="70"/>
+      <c r="FS8" s="70"/>
+      <c r="FT8" s="70"/>
+      <c r="FU8" s="70"/>
+      <c r="FV8" s="70"/>
+      <c r="FW8" s="70"/>
+      <c r="FX8" s="70"/>
+      <c r="FY8" s="70"/>
+      <c r="FZ8" s="70"/>
+      <c r="GA8" s="70"/>
+      <c r="GB8" s="70"/>
+      <c r="GC8" s="70"/>
+      <c r="GD8" s="70"/>
+      <c r="GE8" s="70"/>
+      <c r="GF8" s="70"/>
+      <c r="GG8" s="70"/>
+      <c r="GH8" s="70"/>
+      <c r="GI8" s="70"/>
+      <c r="GJ8" s="70"/>
+      <c r="GK8" s="70"/>
+      <c r="GL8" s="70"/>
+      <c r="GM8" s="70"/>
+      <c r="GN8" s="70"/>
+      <c r="GO8" s="70"/>
+      <c r="GP8" s="70"/>
+      <c r="GQ8" s="70"/>
+      <c r="GR8" s="70"/>
+      <c r="GS8" s="70"/>
+      <c r="GT8" s="70"/>
+      <c r="GU8" s="70"/>
+      <c r="GV8" s="70"/>
+      <c r="GW8" s="70"/>
+      <c r="GX8" s="70"/>
+      <c r="GY8" s="70"/>
+      <c r="GZ8" s="70"/>
+      <c r="HA8" s="70"/>
+      <c r="HB8" s="70"/>
+      <c r="HC8" s="71"/>
     </row>
     <row r="9" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B9" s="32"/>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
-      <c r="E9" s="50"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="32"/>
       <c r="G9" s="33"/>
       <c r="H9" s="34"/>
-      <c r="I9" s="46"/>
-      <c r="J9" s="68"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="67"/>
     </row>
     <row r="10" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
       <c r="C10" s="33"/>
       <c r="D10" s="33"/>
-      <c r="E10" s="50"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="32"/>
       <c r="G10" s="33"/>
       <c r="H10" s="34"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="68"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="67"/>
     </row>
     <row r="11" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B11" s="32"/>
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
-      <c r="E11" s="50"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="32"/>
       <c r="G11" s="33"/>
       <c r="H11" s="34"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="68"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="67"/>
     </row>
     <row r="12" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B12" s="32"/>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
-      <c r="E12" s="50"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
       <c r="H12" s="34"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="68"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="67"/>
     </row>
     <row r="13" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B13" s="32"/>
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
-      <c r="E13" s="50"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
       <c r="H13" s="34"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="68"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="67"/>
     </row>
     <row r="14" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
-      <c r="E14" s="50"/>
+      <c r="E14" s="49"/>
       <c r="F14" s="32"/>
       <c r="G14" s="33"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="68"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="67"/>
     </row>
     <row r="15" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
-      <c r="E15" s="50"/>
+      <c r="E15" s="49"/>
       <c r="F15" s="32"/>
       <c r="G15" s="33"/>
       <c r="H15" s="34"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="68"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="67"/>
     </row>
     <row r="16" spans="1:211" x14ac:dyDescent="0.25">
       <c r="B16" s="32"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
-      <c r="E16" s="50"/>
+      <c r="E16" s="49"/>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
       <c r="H16" s="34"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="68"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="67"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="32"/>
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
-      <c r="E17" s="50"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
       <c r="H17" s="34"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="68"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="67"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="32"/>
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
-      <c r="E18" s="50"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
       <c r="H18" s="34"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="68"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="67"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
-      <c r="E19" s="50"/>
+      <c r="E19" s="49"/>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="34"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="68"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="67"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
-      <c r="E20" s="50"/>
+      <c r="E20" s="49"/>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="34"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="68"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="67"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
-      <c r="E21" s="50"/>
+      <c r="E21" s="49"/>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
       <c r="H21" s="34"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="68"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="67"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
-      <c r="E22" s="50"/>
+      <c r="E22" s="49"/>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
       <c r="H22" s="34"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="68"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="67"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="32"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
-      <c r="E23" s="50"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
       <c r="H23" s="34"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="68"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="67"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="32"/>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
-      <c r="E24" s="50"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
       <c r="H24" s="34"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="68"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="67"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="32"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
-      <c r="E25" s="50"/>
+      <c r="E25" s="49"/>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
       <c r="H25" s="34"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="68"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="67"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="32"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
-      <c r="E26" s="50"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
       <c r="H26" s="34"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="68"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="67"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="32"/>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
-      <c r="E27" s="50"/>
+      <c r="E27" s="49"/>
       <c r="F27" s="32"/>
       <c r="G27" s="33"/>
       <c r="H27" s="34"/>
-      <c r="I27" s="46"/>
-      <c r="J27" s="68"/>
+      <c r="I27" s="45"/>
+      <c r="J27" s="67"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
-      <c r="E28" s="50"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="32"/>
       <c r="G28" s="33"/>
       <c r="H28" s="34"/>
-      <c r="I28" s="46"/>
-      <c r="J28" s="68"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="67"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="32"/>
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
-      <c r="E29" s="50"/>
+      <c r="E29" s="49"/>
       <c r="F29" s="32"/>
       <c r="G29" s="33"/>
       <c r="H29" s="34"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="68"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="67"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="32"/>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
-      <c r="E30" s="50"/>
+      <c r="E30" s="49"/>
       <c r="F30" s="32"/>
       <c r="G30" s="33"/>
       <c r="H30" s="34"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="68"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="67"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="32"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
-      <c r="E31" s="50"/>
+      <c r="E31" s="49"/>
       <c r="F31" s="32"/>
       <c r="G31" s="33"/>
       <c r="H31" s="34"/>
-      <c r="I31" s="46"/>
-      <c r="J31" s="68"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="67"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="32"/>
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
-      <c r="E32" s="50"/>
+      <c r="E32" s="49"/>
       <c r="F32" s="32"/>
       <c r="G32" s="33"/>
       <c r="H32" s="34"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="68"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="67"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="32"/>
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
-      <c r="E33" s="50"/>
+      <c r="E33" s="49"/>
       <c r="F33" s="32"/>
       <c r="G33" s="33"/>
       <c r="H33" s="34"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="68"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="67"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="32"/>
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
-      <c r="E34" s="50"/>
+      <c r="E34" s="49"/>
       <c r="F34" s="32"/>
       <c r="G34" s="33"/>
       <c r="H34" s="34"/>
-      <c r="I34" s="46"/>
-      <c r="J34" s="68"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="67"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="32"/>
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
-      <c r="E35" s="50"/>
+      <c r="E35" s="49"/>
       <c r="F35" s="32"/>
       <c r="G35" s="33"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="46"/>
-      <c r="J35" s="68"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="67"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="32"/>
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
-      <c r="E36" s="50"/>
+      <c r="E36" s="49"/>
       <c r="F36" s="32"/>
       <c r="G36" s="33"/>
       <c r="H36" s="34"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="68"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="67"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
-      <c r="E37" s="50"/>
+      <c r="E37" s="49"/>
       <c r="F37" s="32"/>
       <c r="G37" s="33"/>
       <c r="H37" s="34"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="68"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="67"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="32"/>
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
-      <c r="E38" s="50"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="32"/>
       <c r="G38" s="33"/>
       <c r="H38" s="34"/>
-      <c r="I38" s="46"/>
-      <c r="J38" s="68"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="67"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="32"/>
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
-      <c r="E39" s="50"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="32"/>
       <c r="G39" s="33"/>
       <c r="H39" s="34"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="68"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="67"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="32"/>
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
-      <c r="E40" s="50"/>
+      <c r="E40" s="49"/>
       <c r="F40" s="32"/>
       <c r="G40" s="33"/>
       <c r="H40" s="34"/>
-      <c r="I40" s="46"/>
-      <c r="J40" s="68"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="67"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="32"/>
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
-      <c r="E41" s="50"/>
+      <c r="E41" s="49"/>
       <c r="F41" s="32"/>
       <c r="G41" s="33"/>
       <c r="H41" s="34"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="68"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="67"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
-      <c r="E42" s="50"/>
+      <c r="E42" s="49"/>
       <c r="F42" s="32"/>
       <c r="G42" s="33"/>
       <c r="H42" s="34"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="68"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="67"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
-      <c r="E43" s="50"/>
+      <c r="E43" s="49"/>
       <c r="F43" s="32"/>
       <c r="G43" s="33"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="46"/>
-      <c r="J43" s="68"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="67"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
-      <c r="E44" s="50"/>
+      <c r="E44" s="49"/>
       <c r="F44" s="32"/>
       <c r="G44" s="33"/>
       <c r="H44" s="34"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="68"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="67"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
-      <c r="E45" s="50"/>
+      <c r="E45" s="49"/>
       <c r="F45" s="32"/>
       <c r="G45" s="33"/>
       <c r="H45" s="34"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="68"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="67"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="32"/>
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
-      <c r="E46" s="50"/>
+      <c r="E46" s="49"/>
       <c r="F46" s="32"/>
       <c r="G46" s="33"/>
       <c r="H46" s="34"/>
-      <c r="I46" s="46"/>
-      <c r="J46" s="68"/>
+      <c r="I46" s="45"/>
+      <c r="J46" s="67"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="32"/>
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
-      <c r="E47" s="50"/>
+      <c r="E47" s="49"/>
       <c r="F47" s="32"/>
       <c r="G47" s="33"/>
       <c r="H47" s="34"/>
-      <c r="I47" s="46"/>
-      <c r="J47" s="68"/>
+      <c r="I47" s="45"/>
+      <c r="J47" s="67"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="32"/>
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
-      <c r="E48" s="50"/>
+      <c r="E48" s="49"/>
       <c r="F48" s="32"/>
       <c r="G48" s="33"/>
       <c r="H48" s="34"/>
-      <c r="I48" s="46"/>
-      <c r="J48" s="68"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="67"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" s="32"/>
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
-      <c r="E49" s="50"/>
+      <c r="E49" s="49"/>
       <c r="F49" s="32"/>
       <c r="G49" s="33"/>
       <c r="H49" s="34"/>
-      <c r="I49" s="46"/>
-      <c r="J49" s="68"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="67"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="32"/>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
-      <c r="E50" s="50"/>
+      <c r="E50" s="49"/>
       <c r="F50" s="32"/>
       <c r="G50" s="33"/>
       <c r="H50" s="34"/>
-      <c r="I50" s="46"/>
-      <c r="J50" s="68"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="67"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="32"/>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
-      <c r="E51" s="50"/>
+      <c r="E51" s="49"/>
       <c r="F51" s="32"/>
       <c r="G51" s="33"/>
       <c r="H51" s="34"/>
-      <c r="I51" s="46"/>
-      <c r="J51" s="68"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="67"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="32"/>
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
-      <c r="E52" s="50"/>
+      <c r="E52" s="49"/>
       <c r="F52" s="32"/>
       <c r="G52" s="33"/>
       <c r="H52" s="34"/>
-      <c r="I52" s="46"/>
-      <c r="J52" s="68"/>
+      <c r="I52" s="45"/>
+      <c r="J52" s="67"/>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="32"/>
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
-      <c r="E53" s="50"/>
+      <c r="E53" s="49"/>
       <c r="F53" s="32"/>
       <c r="G53" s="33"/>
       <c r="H53" s="34"/>
-      <c r="I53" s="46"/>
-      <c r="J53" s="68"/>
+      <c r="I53" s="45"/>
+      <c r="J53" s="67"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="32"/>
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
-      <c r="E54" s="50"/>
+      <c r="E54" s="49"/>
       <c r="F54" s="32"/>
       <c r="G54" s="33"/>
       <c r="H54" s="34"/>
-      <c r="I54" s="46"/>
-      <c r="J54" s="68"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="67"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" s="32"/>
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
-      <c r="E55" s="50"/>
+      <c r="E55" s="49"/>
       <c r="F55" s="32"/>
       <c r="G55" s="33"/>
       <c r="H55" s="34"/>
-      <c r="I55" s="46"/>
-      <c r="J55" s="68"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="67"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="32"/>
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
-      <c r="E56" s="50"/>
+      <c r="E56" s="49"/>
       <c r="F56" s="32"/>
       <c r="G56" s="33"/>
       <c r="H56" s="34"/>
-      <c r="I56" s="46"/>
-      <c r="J56" s="68"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="67"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="32"/>
       <c r="C57" s="33"/>
       <c r="D57" s="33"/>
-      <c r="E57" s="50"/>
+      <c r="E57" s="49"/>
       <c r="F57" s="32"/>
       <c r="G57" s="33"/>
       <c r="H57" s="34"/>
       <c r="I57" s="32"/>
-      <c r="J57" s="68"/>
+      <c r="J57" s="67"/>
     </row>
     <row r="1048575" spans="12:211" x14ac:dyDescent="0.25">
-      <c r="L1048575" s="48"/>
-      <c r="M1048575" s="41"/>
-      <c r="N1048575" s="41"/>
-      <c r="O1048575" s="41"/>
-      <c r="P1048575" s="41"/>
-      <c r="Q1048575" s="41"/>
-      <c r="R1048575" s="41"/>
-      <c r="S1048575" s="41"/>
-      <c r="T1048575" s="41"/>
-      <c r="U1048575" s="41"/>
-      <c r="V1048575" s="41"/>
-      <c r="W1048575" s="41"/>
-      <c r="X1048575" s="41"/>
-      <c r="Y1048575" s="41"/>
-      <c r="Z1048575" s="41"/>
-      <c r="AA1048575" s="41"/>
-      <c r="AB1048575" s="41"/>
-      <c r="AC1048575" s="41"/>
-      <c r="AD1048575" s="41"/>
-      <c r="AE1048575" s="41"/>
-      <c r="AF1048575" s="41"/>
-      <c r="AG1048575" s="41"/>
-      <c r="AH1048575" s="41"/>
-      <c r="AI1048575" s="41"/>
-      <c r="AJ1048575" s="41"/>
-      <c r="AK1048575" s="41"/>
-      <c r="AL1048575" s="41"/>
-      <c r="AM1048575" s="41"/>
-      <c r="AN1048575" s="41"/>
-      <c r="AO1048575" s="41"/>
-      <c r="AP1048575" s="41"/>
-      <c r="AQ1048575" s="41"/>
-      <c r="AR1048575" s="41"/>
-      <c r="AS1048575" s="41"/>
-      <c r="AT1048575" s="41"/>
-      <c r="AU1048575" s="41"/>
-      <c r="AV1048575" s="41"/>
-      <c r="AW1048575" s="41"/>
-      <c r="AX1048575" s="41"/>
-      <c r="AY1048575" s="41"/>
-      <c r="AZ1048575" s="41"/>
-      <c r="BA1048575" s="41"/>
-      <c r="BB1048575" s="41"/>
-      <c r="BC1048575" s="41"/>
-      <c r="BD1048575" s="41"/>
-      <c r="BE1048575" s="41"/>
-      <c r="BF1048575" s="41"/>
-      <c r="BG1048575" s="41"/>
-      <c r="BH1048575" s="41"/>
-      <c r="BI1048575" s="41"/>
-      <c r="BJ1048575" s="41"/>
-      <c r="BK1048575" s="41"/>
-      <c r="BL1048575" s="41"/>
-      <c r="BM1048575" s="41"/>
-      <c r="BN1048575" s="41"/>
-      <c r="BO1048575" s="41"/>
-      <c r="BP1048575" s="41"/>
-      <c r="BQ1048575" s="41"/>
-      <c r="BR1048575" s="41"/>
-      <c r="BS1048575" s="41"/>
-      <c r="BT1048575" s="41"/>
-      <c r="BU1048575" s="41"/>
-      <c r="BV1048575" s="41"/>
-      <c r="BW1048575" s="41"/>
-      <c r="BX1048575" s="41"/>
-      <c r="BY1048575" s="41"/>
-      <c r="BZ1048575" s="41"/>
-      <c r="CA1048575" s="41"/>
-      <c r="CB1048575" s="41"/>
-      <c r="CC1048575" s="41"/>
-      <c r="CD1048575" s="41"/>
-      <c r="CE1048575" s="41"/>
-      <c r="CF1048575" s="41"/>
-      <c r="CG1048575" s="41"/>
-      <c r="CH1048575" s="41"/>
-      <c r="CI1048575" s="41"/>
-      <c r="CJ1048575" s="41"/>
-      <c r="CK1048575" s="41"/>
-      <c r="CL1048575" s="41"/>
-      <c r="CM1048575" s="41"/>
-      <c r="CN1048575" s="41"/>
-      <c r="CO1048575" s="41"/>
-      <c r="CP1048575" s="41"/>
-      <c r="CQ1048575" s="41"/>
-      <c r="CR1048575" s="41"/>
-      <c r="CS1048575" s="41"/>
-      <c r="CT1048575" s="41"/>
-      <c r="CU1048575" s="41"/>
-      <c r="CV1048575" s="41"/>
-      <c r="CW1048575" s="41"/>
-      <c r="CX1048575" s="41"/>
-      <c r="CY1048575" s="41"/>
-      <c r="CZ1048575" s="41"/>
-      <c r="DA1048575" s="41"/>
-      <c r="DB1048575" s="41"/>
-      <c r="DC1048575" s="41"/>
-      <c r="DD1048575" s="41"/>
-      <c r="DE1048575" s="41"/>
-      <c r="DF1048575" s="41"/>
-      <c r="DG1048575" s="41"/>
-      <c r="DH1048575" s="41"/>
-      <c r="DI1048575" s="41"/>
-      <c r="DJ1048575" s="41"/>
-      <c r="DK1048575" s="41"/>
-      <c r="DL1048575" s="41"/>
-      <c r="DM1048575" s="41"/>
-      <c r="DN1048575" s="41"/>
-      <c r="DO1048575" s="41"/>
-      <c r="DP1048575" s="41"/>
-      <c r="DQ1048575" s="41"/>
-      <c r="DR1048575" s="41"/>
-      <c r="DS1048575" s="41"/>
-      <c r="DT1048575" s="41"/>
-      <c r="DU1048575" s="41"/>
-      <c r="DV1048575" s="41"/>
-      <c r="DW1048575" s="41"/>
-      <c r="DX1048575" s="41"/>
-      <c r="DY1048575" s="41"/>
-      <c r="DZ1048575" s="41"/>
-      <c r="EA1048575" s="41"/>
-      <c r="EB1048575" s="41"/>
-      <c r="EC1048575" s="41"/>
-      <c r="ED1048575" s="41"/>
-      <c r="EE1048575" s="41"/>
-      <c r="EF1048575" s="41"/>
-      <c r="EG1048575" s="41"/>
-      <c r="EH1048575" s="41"/>
-      <c r="EI1048575" s="41"/>
-      <c r="EJ1048575" s="41"/>
-      <c r="EK1048575" s="41"/>
-      <c r="EL1048575" s="41"/>
-      <c r="EM1048575" s="41"/>
-      <c r="EN1048575" s="41"/>
-      <c r="EO1048575" s="41"/>
-      <c r="EP1048575" s="41"/>
-      <c r="EQ1048575" s="41"/>
-      <c r="ER1048575" s="41"/>
-      <c r="ES1048575" s="41"/>
-      <c r="ET1048575" s="41"/>
-      <c r="EU1048575" s="41"/>
-      <c r="EV1048575" s="41"/>
-      <c r="EW1048575" s="41"/>
-      <c r="EX1048575" s="41"/>
-      <c r="EY1048575" s="41"/>
-      <c r="EZ1048575" s="41"/>
-      <c r="FA1048575" s="41"/>
-      <c r="FB1048575" s="41"/>
-      <c r="FC1048575" s="41"/>
-      <c r="FD1048575" s="41"/>
-      <c r="FE1048575" s="41"/>
-      <c r="FF1048575" s="41"/>
-      <c r="FG1048575" s="41"/>
-      <c r="FH1048575" s="41"/>
-      <c r="FI1048575" s="41"/>
-      <c r="FJ1048575" s="41"/>
-      <c r="FK1048575" s="41"/>
-      <c r="FL1048575" s="41"/>
-      <c r="FM1048575" s="41"/>
-      <c r="FN1048575" s="41"/>
-      <c r="FO1048575" s="41"/>
-      <c r="FP1048575" s="41"/>
-      <c r="FQ1048575" s="41"/>
-      <c r="FR1048575" s="41"/>
-      <c r="FS1048575" s="41"/>
-      <c r="FT1048575" s="41"/>
-      <c r="FU1048575" s="41"/>
-      <c r="FV1048575" s="41"/>
-      <c r="FW1048575" s="41"/>
-      <c r="FX1048575" s="41"/>
-      <c r="FY1048575" s="41"/>
-      <c r="FZ1048575" s="41"/>
-      <c r="GA1048575" s="41"/>
-      <c r="GB1048575" s="41"/>
-      <c r="GC1048575" s="41"/>
-      <c r="GD1048575" s="41"/>
-      <c r="GE1048575" s="41"/>
-      <c r="GF1048575" s="41"/>
-      <c r="GG1048575" s="41"/>
-      <c r="GH1048575" s="41"/>
-      <c r="GI1048575" s="41"/>
-      <c r="GJ1048575" s="41"/>
-      <c r="GK1048575" s="41"/>
-      <c r="GL1048575" s="41"/>
-      <c r="GM1048575" s="41"/>
-      <c r="GN1048575" s="41"/>
-      <c r="GO1048575" s="41"/>
-      <c r="GP1048575" s="41"/>
-      <c r="GQ1048575" s="41"/>
-      <c r="GR1048575" s="41"/>
-      <c r="GS1048575" s="41"/>
-      <c r="GT1048575" s="41"/>
-      <c r="GU1048575" s="41"/>
-      <c r="GV1048575" s="41"/>
-      <c r="GW1048575" s="41"/>
-      <c r="GX1048575" s="41"/>
-      <c r="GY1048575" s="41"/>
-      <c r="GZ1048575" s="41"/>
-      <c r="HA1048575" s="41"/>
-      <c r="HB1048575" s="41"/>
-      <c r="HC1048575" s="47"/>
+      <c r="L1048575" s="47"/>
+      <c r="M1048575" s="40"/>
+      <c r="N1048575" s="40"/>
+      <c r="O1048575" s="40"/>
+      <c r="P1048575" s="40"/>
+      <c r="Q1048575" s="40"/>
+      <c r="R1048575" s="40"/>
+      <c r="S1048575" s="40"/>
+      <c r="T1048575" s="40"/>
+      <c r="U1048575" s="40"/>
+      <c r="V1048575" s="40"/>
+      <c r="W1048575" s="40"/>
+      <c r="X1048575" s="40"/>
+      <c r="Y1048575" s="40"/>
+      <c r="Z1048575" s="40"/>
+      <c r="AA1048575" s="40"/>
+      <c r="AB1048575" s="40"/>
+      <c r="AC1048575" s="40"/>
+      <c r="AD1048575" s="40"/>
+      <c r="AE1048575" s="40"/>
+      <c r="AF1048575" s="40"/>
+      <c r="AG1048575" s="40"/>
+      <c r="AH1048575" s="40"/>
+      <c r="AI1048575" s="40"/>
+      <c r="AJ1048575" s="40"/>
+      <c r="AK1048575" s="40"/>
+      <c r="AL1048575" s="40"/>
+      <c r="AM1048575" s="40"/>
+      <c r="AN1048575" s="40"/>
+      <c r="AO1048575" s="40"/>
+      <c r="AP1048575" s="40"/>
+      <c r="AQ1048575" s="40"/>
+      <c r="AR1048575" s="40"/>
+      <c r="AS1048575" s="40"/>
+      <c r="AT1048575" s="40"/>
+      <c r="AU1048575" s="40"/>
+      <c r="AV1048575" s="40"/>
+      <c r="AW1048575" s="40"/>
+      <c r="AX1048575" s="40"/>
+      <c r="AY1048575" s="40"/>
+      <c r="AZ1048575" s="40"/>
+      <c r="BA1048575" s="40"/>
+      <c r="BB1048575" s="40"/>
+      <c r="BC1048575" s="40"/>
+      <c r="BD1048575" s="40"/>
+      <c r="BE1048575" s="40"/>
+      <c r="BF1048575" s="40"/>
+      <c r="BG1048575" s="40"/>
+      <c r="BH1048575" s="40"/>
+      <c r="BI1048575" s="40"/>
+      <c r="BJ1048575" s="40"/>
+      <c r="BK1048575" s="40"/>
+      <c r="BL1048575" s="40"/>
+      <c r="BM1048575" s="40"/>
+      <c r="BN1048575" s="40"/>
+      <c r="BO1048575" s="40"/>
+      <c r="BP1048575" s="40"/>
+      <c r="BQ1048575" s="40"/>
+      <c r="BR1048575" s="40"/>
+      <c r="BS1048575" s="40"/>
+      <c r="BT1048575" s="40"/>
+      <c r="BU1048575" s="40"/>
+      <c r="BV1048575" s="40"/>
+      <c r="BW1048575" s="40"/>
+      <c r="BX1048575" s="40"/>
+      <c r="BY1048575" s="40"/>
+      <c r="BZ1048575" s="40"/>
+      <c r="CA1048575" s="40"/>
+      <c r="CB1048575" s="40"/>
+      <c r="CC1048575" s="40"/>
+      <c r="CD1048575" s="40"/>
+      <c r="CE1048575" s="40"/>
+      <c r="CF1048575" s="40"/>
+      <c r="CG1048575" s="40"/>
+      <c r="CH1048575" s="40"/>
+      <c r="CI1048575" s="40"/>
+      <c r="CJ1048575" s="40"/>
+      <c r="CK1048575" s="40"/>
+      <c r="CL1048575" s="40"/>
+      <c r="CM1048575" s="40"/>
+      <c r="CN1048575" s="40"/>
+      <c r="CO1048575" s="40"/>
+      <c r="CP1048575" s="40"/>
+      <c r="CQ1048575" s="40"/>
+      <c r="CR1048575" s="40"/>
+      <c r="CS1048575" s="40"/>
+      <c r="CT1048575" s="40"/>
+      <c r="CU1048575" s="40"/>
+      <c r="CV1048575" s="40"/>
+      <c r="CW1048575" s="40"/>
+      <c r="CX1048575" s="40"/>
+      <c r="CY1048575" s="40"/>
+      <c r="CZ1048575" s="40"/>
+      <c r="DA1048575" s="40"/>
+      <c r="DB1048575" s="40"/>
+      <c r="DC1048575" s="40"/>
+      <c r="DD1048575" s="40"/>
+      <c r="DE1048575" s="40"/>
+      <c r="DF1048575" s="40"/>
+      <c r="DG1048575" s="40"/>
+      <c r="DH1048575" s="40"/>
+      <c r="DI1048575" s="40"/>
+      <c r="DJ1048575" s="40"/>
+      <c r="DK1048575" s="40"/>
+      <c r="DL1048575" s="40"/>
+      <c r="DM1048575" s="40"/>
+      <c r="DN1048575" s="40"/>
+      <c r="DO1048575" s="40"/>
+      <c r="DP1048575" s="40"/>
+      <c r="DQ1048575" s="40"/>
+      <c r="DR1048575" s="40"/>
+      <c r="DS1048575" s="40"/>
+      <c r="DT1048575" s="40"/>
+      <c r="DU1048575" s="40"/>
+      <c r="DV1048575" s="40"/>
+      <c r="DW1048575" s="40"/>
+      <c r="DX1048575" s="40"/>
+      <c r="DY1048575" s="40"/>
+      <c r="DZ1048575" s="40"/>
+      <c r="EA1048575" s="40"/>
+      <c r="EB1048575" s="40"/>
+      <c r="EC1048575" s="40"/>
+      <c r="ED1048575" s="40"/>
+      <c r="EE1048575" s="40"/>
+      <c r="EF1048575" s="40"/>
+      <c r="EG1048575" s="40"/>
+      <c r="EH1048575" s="40"/>
+      <c r="EI1048575" s="40"/>
+      <c r="EJ1048575" s="40"/>
+      <c r="EK1048575" s="40"/>
+      <c r="EL1048575" s="40"/>
+      <c r="EM1048575" s="40"/>
+      <c r="EN1048575" s="40"/>
+      <c r="EO1048575" s="40"/>
+      <c r="EP1048575" s="40"/>
+      <c r="EQ1048575" s="40"/>
+      <c r="ER1048575" s="40"/>
+      <c r="ES1048575" s="40"/>
+      <c r="ET1048575" s="40"/>
+      <c r="EU1048575" s="40"/>
+      <c r="EV1048575" s="40"/>
+      <c r="EW1048575" s="40"/>
+      <c r="EX1048575" s="40"/>
+      <c r="EY1048575" s="40"/>
+      <c r="EZ1048575" s="40"/>
+      <c r="FA1048575" s="40"/>
+      <c r="FB1048575" s="40"/>
+      <c r="FC1048575" s="40"/>
+      <c r="FD1048575" s="40"/>
+      <c r="FE1048575" s="40"/>
+      <c r="FF1048575" s="40"/>
+      <c r="FG1048575" s="40"/>
+      <c r="FH1048575" s="40"/>
+      <c r="FI1048575" s="40"/>
+      <c r="FJ1048575" s="40"/>
+      <c r="FK1048575" s="40"/>
+      <c r="FL1048575" s="40"/>
+      <c r="FM1048575" s="40"/>
+      <c r="FN1048575" s="40"/>
+      <c r="FO1048575" s="40"/>
+      <c r="FP1048575" s="40"/>
+      <c r="FQ1048575" s="40"/>
+      <c r="FR1048575" s="40"/>
+      <c r="FS1048575" s="40"/>
+      <c r="FT1048575" s="40"/>
+      <c r="FU1048575" s="40"/>
+      <c r="FV1048575" s="40"/>
+      <c r="FW1048575" s="40"/>
+      <c r="FX1048575" s="40"/>
+      <c r="FY1048575" s="40"/>
+      <c r="FZ1048575" s="40"/>
+      <c r="GA1048575" s="40"/>
+      <c r="GB1048575" s="40"/>
+      <c r="GC1048575" s="40"/>
+      <c r="GD1048575" s="40"/>
+      <c r="GE1048575" s="40"/>
+      <c r="GF1048575" s="40"/>
+      <c r="GG1048575" s="40"/>
+      <c r="GH1048575" s="40"/>
+      <c r="GI1048575" s="40"/>
+      <c r="GJ1048575" s="40"/>
+      <c r="GK1048575" s="40"/>
+      <c r="GL1048575" s="40"/>
+      <c r="GM1048575" s="40"/>
+      <c r="GN1048575" s="40"/>
+      <c r="GO1048575" s="40"/>
+      <c r="GP1048575" s="40"/>
+      <c r="GQ1048575" s="40"/>
+      <c r="GR1048575" s="40"/>
+      <c r="GS1048575" s="40"/>
+      <c r="GT1048575" s="40"/>
+      <c r="GU1048575" s="40"/>
+      <c r="GV1048575" s="40"/>
+      <c r="GW1048575" s="40"/>
+      <c r="GX1048575" s="40"/>
+      <c r="GY1048575" s="40"/>
+      <c r="GZ1048575" s="40"/>
+      <c r="HA1048575" s="40"/>
+      <c r="HB1048575" s="40"/>
+      <c r="HC1048575" s="46"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="7y30xUDt19rWnUkEQecomBB6U3TesPo1zIQt5KuetdcxPNveuCy0au6mtZqQUzv9gQBEfL6GPDrN1yO8U17XeA==" saltValue="PQ1Y3bVNWcuOHWop+u1utg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>

</xml_diff>

<commit_message>
Review and edits in most forms
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1DI.xlsx
+++ b/form_reporting_templates/Form-1DI.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6468A58C-C8D8-427A-A2B5-EBF610DA836F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4792399-A0F1-4C93-8701-8A4969D7A8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
-  <si>
-    <t>Focal point</t>
-  </si>
   <si>
     <t>Name</t>
   </si>
@@ -168,14 +165,17 @@
   <si>
     <t>Main elements</t>
   </si>
+  <si>
+    <t>Liaison officer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -795,10 +795,10 @@
   <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1035,6 +1035,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1136,10 +1140,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1473,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,39 +1489,39 @@
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="83" t="s">
-        <v>31</v>
+      <c r="B2" s="84" t="s">
+        <v>30</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86"/>
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="88"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="89"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="8"/>
     </row>
@@ -1537,7 +1537,7 @@
     <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="9"/>
       <c r="C6" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -1556,26 +1556,26 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="9"/>
-      <c r="C8" s="82" t="s">
-        <v>0</v>
+      <c r="C8" s="83" t="s">
+        <v>34</v>
       </c>
-      <c r="D8" s="82"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="82" t="s">
-        <v>26</v>
+      <c r="F8" s="83" t="s">
+        <v>25</v>
       </c>
-      <c r="G8" s="82"/>
+      <c r="G8" s="83"/>
       <c r="H8" s="11"/>
     </row>
     <row r="9" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="10"/>
       <c r="F9" s="13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="11"/>
@@ -1583,12 +1583,12 @@
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="9"/>
       <c r="C10" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="24"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="11"/>
@@ -1605,9 +1605,9 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="9"/>
       <c r="C12" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
-      <c r="D12" s="112"/>
+      <c r="D12" s="79"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -1616,9 +1616,9 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
-      <c r="D13" s="112"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1645,7 +1645,7 @@
     <row r="16" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="9"/>
       <c r="C16" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1665,7 +1665,7 @@
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="9"/>
       <c r="C18" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="39"/>
       <c r="E18" s="10"/>
@@ -1676,7 +1676,7 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="9"/>
       <c r="C19" s="51" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="10"/>
@@ -1687,7 +1687,7 @@
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="C20" s="77" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="39"/>
       <c r="E20" s="10"/>
@@ -1716,7 +1716,7 @@
     <row r="23" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="9"/>
       <c r="C23" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="10"/>
@@ -1735,11 +1735,11 @@
     </row>
     <row r="25" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="81"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
       <c r="H25" s="11"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1756,7 +1756,7 @@
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qzzWBlZZUVBt3RoNQOKuUOqB4TFmwsWjMhr2d3TjT7WEcJJt/O6k8cSlBfdipxgawf2q30/RSpWug0+BawY5pw==" saltValue="8HpRcGRg8db+djtBnAW3fw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7U7/Qt/9oOtBEff6qv3dYDnEa1ebiJlsXJoJOPJWthLKwyFXhTQmUxAB8ybSQNAAbfVsXr3lqKewQd/wnoKImg==" saltValue="2Pzu5Tizz9+r1G0lldUyRg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>
@@ -1781,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:HC1048575"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="11" ySplit="7" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -1811,18 +1811,18 @@
       <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="83" t="s">
-        <v>32</v>
+      <c r="B2" s="84" t="s">
+        <v>31</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="110"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="111"/>
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
       <c r="N2" s="35"/>
@@ -2026,237 +2026,237 @@
     </row>
     <row r="3" spans="1:211" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="107" t="s">
-        <v>25</v>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="108" t="s">
+        <v>24</v>
       </c>
-      <c r="M3" s="108"/>
-      <c r="N3" s="108"/>
-      <c r="O3" s="108"/>
-      <c r="P3" s="108"/>
-      <c r="Q3" s="108"/>
-      <c r="R3" s="108"/>
-      <c r="S3" s="108"/>
-      <c r="T3" s="108"/>
-      <c r="U3" s="108"/>
-      <c r="V3" s="108"/>
-      <c r="W3" s="108"/>
-      <c r="X3" s="108"/>
-      <c r="Y3" s="108"/>
-      <c r="Z3" s="108"/>
-      <c r="AA3" s="108"/>
-      <c r="AB3" s="108"/>
-      <c r="AC3" s="108"/>
-      <c r="AD3" s="108"/>
-      <c r="AE3" s="108"/>
-      <c r="AF3" s="108"/>
-      <c r="AG3" s="108"/>
-      <c r="AH3" s="108"/>
-      <c r="AI3" s="108"/>
-      <c r="AJ3" s="108"/>
-      <c r="AK3" s="108"/>
-      <c r="AL3" s="108"/>
-      <c r="AM3" s="108"/>
-      <c r="AN3" s="108"/>
-      <c r="AO3" s="108"/>
-      <c r="AP3" s="108"/>
-      <c r="AQ3" s="108"/>
-      <c r="AR3" s="108"/>
-      <c r="AS3" s="108"/>
-      <c r="AT3" s="108"/>
-      <c r="AU3" s="108"/>
-      <c r="AV3" s="108"/>
-      <c r="AW3" s="108"/>
-      <c r="AX3" s="108"/>
-      <c r="AY3" s="108"/>
-      <c r="AZ3" s="108"/>
-      <c r="BA3" s="108"/>
-      <c r="BB3" s="108"/>
-      <c r="BC3" s="108"/>
-      <c r="BD3" s="108"/>
-      <c r="BE3" s="108"/>
-      <c r="BF3" s="108"/>
-      <c r="BG3" s="108"/>
-      <c r="BH3" s="108"/>
-      <c r="BI3" s="108"/>
-      <c r="BJ3" s="108"/>
-      <c r="BK3" s="108"/>
-      <c r="BL3" s="108"/>
-      <c r="BM3" s="108"/>
-      <c r="BN3" s="108"/>
-      <c r="BO3" s="108"/>
-      <c r="BP3" s="108"/>
-      <c r="BQ3" s="108"/>
-      <c r="BR3" s="108"/>
-      <c r="BS3" s="108"/>
-      <c r="BT3" s="108"/>
-      <c r="BU3" s="108"/>
-      <c r="BV3" s="108"/>
-      <c r="BW3" s="108"/>
-      <c r="BX3" s="108"/>
-      <c r="BY3" s="108"/>
-      <c r="BZ3" s="108"/>
-      <c r="CA3" s="108"/>
-      <c r="CB3" s="108"/>
-      <c r="CC3" s="108"/>
-      <c r="CD3" s="108"/>
-      <c r="CE3" s="108"/>
-      <c r="CF3" s="108"/>
-      <c r="CG3" s="108"/>
-      <c r="CH3" s="108"/>
-      <c r="CI3" s="108"/>
-      <c r="CJ3" s="108"/>
-      <c r="CK3" s="108"/>
-      <c r="CL3" s="108"/>
-      <c r="CM3" s="108"/>
-      <c r="CN3" s="108"/>
-      <c r="CO3" s="108"/>
-      <c r="CP3" s="108"/>
-      <c r="CQ3" s="108"/>
-      <c r="CR3" s="108"/>
-      <c r="CS3" s="108"/>
-      <c r="CT3" s="108"/>
-      <c r="CU3" s="108"/>
-      <c r="CV3" s="108"/>
-      <c r="CW3" s="108"/>
-      <c r="CX3" s="108"/>
-      <c r="CY3" s="108"/>
-      <c r="CZ3" s="108"/>
-      <c r="DA3" s="108"/>
-      <c r="DB3" s="108"/>
-      <c r="DC3" s="108"/>
-      <c r="DD3" s="108"/>
-      <c r="DE3" s="108"/>
-      <c r="DF3" s="108"/>
-      <c r="DG3" s="108"/>
-      <c r="DH3" s="108"/>
-      <c r="DI3" s="108"/>
-      <c r="DJ3" s="108"/>
-      <c r="DK3" s="108"/>
-      <c r="DL3" s="108"/>
-      <c r="DM3" s="108"/>
-      <c r="DN3" s="108"/>
-      <c r="DO3" s="108"/>
-      <c r="DP3" s="108"/>
-      <c r="DQ3" s="108"/>
-      <c r="DR3" s="108"/>
-      <c r="DS3" s="108"/>
-      <c r="DT3" s="108"/>
-      <c r="DU3" s="108"/>
-      <c r="DV3" s="108"/>
-      <c r="DW3" s="108"/>
-      <c r="DX3" s="108"/>
-      <c r="DY3" s="108"/>
-      <c r="DZ3" s="108"/>
-      <c r="EA3" s="108"/>
-      <c r="EB3" s="108"/>
-      <c r="EC3" s="108"/>
-      <c r="ED3" s="108"/>
-      <c r="EE3" s="108"/>
-      <c r="EF3" s="108"/>
-      <c r="EG3" s="108"/>
-      <c r="EH3" s="108"/>
-      <c r="EI3" s="108"/>
-      <c r="EJ3" s="108"/>
-      <c r="EK3" s="108"/>
-      <c r="EL3" s="108"/>
-      <c r="EM3" s="108"/>
-      <c r="EN3" s="108"/>
-      <c r="EO3" s="108"/>
-      <c r="EP3" s="108"/>
-      <c r="EQ3" s="108"/>
-      <c r="ER3" s="108"/>
-      <c r="ES3" s="108"/>
-      <c r="ET3" s="108"/>
-      <c r="EU3" s="108"/>
-      <c r="EV3" s="108"/>
-      <c r="EW3" s="108"/>
-      <c r="EX3" s="108"/>
-      <c r="EY3" s="108"/>
-      <c r="EZ3" s="108"/>
-      <c r="FA3" s="108"/>
-      <c r="FB3" s="108"/>
-      <c r="FC3" s="108"/>
-      <c r="FD3" s="108"/>
-      <c r="FE3" s="108"/>
-      <c r="FF3" s="108"/>
-      <c r="FG3" s="108"/>
-      <c r="FH3" s="108"/>
-      <c r="FI3" s="108"/>
-      <c r="FJ3" s="108"/>
-      <c r="FK3" s="108"/>
-      <c r="FL3" s="108"/>
-      <c r="FM3" s="108"/>
-      <c r="FN3" s="108"/>
-      <c r="FO3" s="108"/>
-      <c r="FP3" s="108"/>
-      <c r="FQ3" s="108"/>
-      <c r="FR3" s="108"/>
-      <c r="FS3" s="108"/>
-      <c r="FT3" s="108"/>
-      <c r="FU3" s="108"/>
-      <c r="FV3" s="108"/>
-      <c r="FW3" s="108"/>
-      <c r="FX3" s="108"/>
-      <c r="FY3" s="108"/>
-      <c r="FZ3" s="108"/>
-      <c r="GA3" s="108"/>
-      <c r="GB3" s="108"/>
-      <c r="GC3" s="108"/>
-      <c r="GD3" s="108"/>
-      <c r="GE3" s="108"/>
-      <c r="GF3" s="108"/>
-      <c r="GG3" s="108"/>
-      <c r="GH3" s="108"/>
-      <c r="GI3" s="108"/>
-      <c r="GJ3" s="108"/>
-      <c r="GK3" s="108"/>
-      <c r="GL3" s="108"/>
-      <c r="GM3" s="108"/>
-      <c r="GN3" s="108"/>
-      <c r="GO3" s="108"/>
-      <c r="GP3" s="108"/>
-      <c r="GQ3" s="108"/>
-      <c r="GR3" s="108"/>
-      <c r="GS3" s="108"/>
-      <c r="GT3" s="108"/>
-      <c r="GU3" s="108"/>
-      <c r="GV3" s="108"/>
-      <c r="GW3" s="108"/>
-      <c r="GX3" s="108"/>
-      <c r="GY3" s="108"/>
-      <c r="GZ3" s="108"/>
-      <c r="HA3" s="108"/>
-      <c r="HB3" s="108"/>
-      <c r="HC3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
+      <c r="P3" s="109"/>
+      <c r="Q3" s="109"/>
+      <c r="R3" s="109"/>
+      <c r="S3" s="109"/>
+      <c r="T3" s="109"/>
+      <c r="U3" s="109"/>
+      <c r="V3" s="109"/>
+      <c r="W3" s="109"/>
+      <c r="X3" s="109"/>
+      <c r="Y3" s="109"/>
+      <c r="Z3" s="109"/>
+      <c r="AA3" s="109"/>
+      <c r="AB3" s="109"/>
+      <c r="AC3" s="109"/>
+      <c r="AD3" s="109"/>
+      <c r="AE3" s="109"/>
+      <c r="AF3" s="109"/>
+      <c r="AG3" s="109"/>
+      <c r="AH3" s="109"/>
+      <c r="AI3" s="109"/>
+      <c r="AJ3" s="109"/>
+      <c r="AK3" s="109"/>
+      <c r="AL3" s="109"/>
+      <c r="AM3" s="109"/>
+      <c r="AN3" s="109"/>
+      <c r="AO3" s="109"/>
+      <c r="AP3" s="109"/>
+      <c r="AQ3" s="109"/>
+      <c r="AR3" s="109"/>
+      <c r="AS3" s="109"/>
+      <c r="AT3" s="109"/>
+      <c r="AU3" s="109"/>
+      <c r="AV3" s="109"/>
+      <c r="AW3" s="109"/>
+      <c r="AX3" s="109"/>
+      <c r="AY3" s="109"/>
+      <c r="AZ3" s="109"/>
+      <c r="BA3" s="109"/>
+      <c r="BB3" s="109"/>
+      <c r="BC3" s="109"/>
+      <c r="BD3" s="109"/>
+      <c r="BE3" s="109"/>
+      <c r="BF3" s="109"/>
+      <c r="BG3" s="109"/>
+      <c r="BH3" s="109"/>
+      <c r="BI3" s="109"/>
+      <c r="BJ3" s="109"/>
+      <c r="BK3" s="109"/>
+      <c r="BL3" s="109"/>
+      <c r="BM3" s="109"/>
+      <c r="BN3" s="109"/>
+      <c r="BO3" s="109"/>
+      <c r="BP3" s="109"/>
+      <c r="BQ3" s="109"/>
+      <c r="BR3" s="109"/>
+      <c r="BS3" s="109"/>
+      <c r="BT3" s="109"/>
+      <c r="BU3" s="109"/>
+      <c r="BV3" s="109"/>
+      <c r="BW3" s="109"/>
+      <c r="BX3" s="109"/>
+      <c r="BY3" s="109"/>
+      <c r="BZ3" s="109"/>
+      <c r="CA3" s="109"/>
+      <c r="CB3" s="109"/>
+      <c r="CC3" s="109"/>
+      <c r="CD3" s="109"/>
+      <c r="CE3" s="109"/>
+      <c r="CF3" s="109"/>
+      <c r="CG3" s="109"/>
+      <c r="CH3" s="109"/>
+      <c r="CI3" s="109"/>
+      <c r="CJ3" s="109"/>
+      <c r="CK3" s="109"/>
+      <c r="CL3" s="109"/>
+      <c r="CM3" s="109"/>
+      <c r="CN3" s="109"/>
+      <c r="CO3" s="109"/>
+      <c r="CP3" s="109"/>
+      <c r="CQ3" s="109"/>
+      <c r="CR3" s="109"/>
+      <c r="CS3" s="109"/>
+      <c r="CT3" s="109"/>
+      <c r="CU3" s="109"/>
+      <c r="CV3" s="109"/>
+      <c r="CW3" s="109"/>
+      <c r="CX3" s="109"/>
+      <c r="CY3" s="109"/>
+      <c r="CZ3" s="109"/>
+      <c r="DA3" s="109"/>
+      <c r="DB3" s="109"/>
+      <c r="DC3" s="109"/>
+      <c r="DD3" s="109"/>
+      <c r="DE3" s="109"/>
+      <c r="DF3" s="109"/>
+      <c r="DG3" s="109"/>
+      <c r="DH3" s="109"/>
+      <c r="DI3" s="109"/>
+      <c r="DJ3" s="109"/>
+      <c r="DK3" s="109"/>
+      <c r="DL3" s="109"/>
+      <c r="DM3" s="109"/>
+      <c r="DN3" s="109"/>
+      <c r="DO3" s="109"/>
+      <c r="DP3" s="109"/>
+      <c r="DQ3" s="109"/>
+      <c r="DR3" s="109"/>
+      <c r="DS3" s="109"/>
+      <c r="DT3" s="109"/>
+      <c r="DU3" s="109"/>
+      <c r="DV3" s="109"/>
+      <c r="DW3" s="109"/>
+      <c r="DX3" s="109"/>
+      <c r="DY3" s="109"/>
+      <c r="DZ3" s="109"/>
+      <c r="EA3" s="109"/>
+      <c r="EB3" s="109"/>
+      <c r="EC3" s="109"/>
+      <c r="ED3" s="109"/>
+      <c r="EE3" s="109"/>
+      <c r="EF3" s="109"/>
+      <c r="EG3" s="109"/>
+      <c r="EH3" s="109"/>
+      <c r="EI3" s="109"/>
+      <c r="EJ3" s="109"/>
+      <c r="EK3" s="109"/>
+      <c r="EL3" s="109"/>
+      <c r="EM3" s="109"/>
+      <c r="EN3" s="109"/>
+      <c r="EO3" s="109"/>
+      <c r="EP3" s="109"/>
+      <c r="EQ3" s="109"/>
+      <c r="ER3" s="109"/>
+      <c r="ES3" s="109"/>
+      <c r="ET3" s="109"/>
+      <c r="EU3" s="109"/>
+      <c r="EV3" s="109"/>
+      <c r="EW3" s="109"/>
+      <c r="EX3" s="109"/>
+      <c r="EY3" s="109"/>
+      <c r="EZ3" s="109"/>
+      <c r="FA3" s="109"/>
+      <c r="FB3" s="109"/>
+      <c r="FC3" s="109"/>
+      <c r="FD3" s="109"/>
+      <c r="FE3" s="109"/>
+      <c r="FF3" s="109"/>
+      <c r="FG3" s="109"/>
+      <c r="FH3" s="109"/>
+      <c r="FI3" s="109"/>
+      <c r="FJ3" s="109"/>
+      <c r="FK3" s="109"/>
+      <c r="FL3" s="109"/>
+      <c r="FM3" s="109"/>
+      <c r="FN3" s="109"/>
+      <c r="FO3" s="109"/>
+      <c r="FP3" s="109"/>
+      <c r="FQ3" s="109"/>
+      <c r="FR3" s="109"/>
+      <c r="FS3" s="109"/>
+      <c r="FT3" s="109"/>
+      <c r="FU3" s="109"/>
+      <c r="FV3" s="109"/>
+      <c r="FW3" s="109"/>
+      <c r="FX3" s="109"/>
+      <c r="FY3" s="109"/>
+      <c r="FZ3" s="109"/>
+      <c r="GA3" s="109"/>
+      <c r="GB3" s="109"/>
+      <c r="GC3" s="109"/>
+      <c r="GD3" s="109"/>
+      <c r="GE3" s="109"/>
+      <c r="GF3" s="109"/>
+      <c r="GG3" s="109"/>
+      <c r="GH3" s="109"/>
+      <c r="GI3" s="109"/>
+      <c r="GJ3" s="109"/>
+      <c r="GK3" s="109"/>
+      <c r="GL3" s="109"/>
+      <c r="GM3" s="109"/>
+      <c r="GN3" s="109"/>
+      <c r="GO3" s="109"/>
+      <c r="GP3" s="109"/>
+      <c r="GQ3" s="109"/>
+      <c r="GR3" s="109"/>
+      <c r="GS3" s="109"/>
+      <c r="GT3" s="109"/>
+      <c r="GU3" s="109"/>
+      <c r="GV3" s="109"/>
+      <c r="GW3" s="109"/>
+      <c r="GX3" s="109"/>
+      <c r="GY3" s="109"/>
+      <c r="GZ3" s="109"/>
+      <c r="HA3" s="109"/>
+      <c r="HB3" s="109"/>
+      <c r="HC3" s="110"/>
     </row>
     <row r="4" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="89" t="s">
-        <v>34</v>
+      <c r="B4" s="90" t="s">
+        <v>33</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="98" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="100"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="99"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="98" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="100"/>
+      <c r="J4" s="101"/>
       <c r="K4" s="60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L4" s="26"/>
       <c r="M4" s="27"/>
@@ -2460,17 +2460,17 @@
       <c r="HC4" s="28"/>
     </row>
     <row r="5" spans="1:211" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="92"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="93"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="103"/>
-      <c r="I5" s="101"/>
-      <c r="J5" s="103"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="102"/>
+      <c r="G5" s="103"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="102"/>
+      <c r="J5" s="104"/>
       <c r="K5" s="50" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L5" s="26"/>
       <c r="M5" s="27"/>
@@ -2674,17 +2674,17 @@
       <c r="HC5" s="28"/>
     </row>
     <row r="6" spans="1:211" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="95"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="106"/>
-      <c r="I6" s="104"/>
-      <c r="J6" s="106"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="105"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="105"/>
+      <c r="J6" s="107"/>
       <c r="K6" s="50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L6" s="26"/>
       <c r="M6" s="27"/>
@@ -2889,34 +2889,34 @@
     </row>
     <row r="7" spans="1:211" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="57" t="s">
-        <v>15</v>
-      </c>
       <c r="I7" s="58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" s="59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" s="61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L7" s="29"/>
       <c r="M7" s="30"/>

</xml_diff>

<commit_message>
Harmonisation of url to the Reference Data Catalogue to reflect the version of the forms (1.0.0) and updates of some urls following the change of domain name from 'biological' to 'biology'
</commit_message>
<xml_diff>
--- a/form_reporting_templates/Form-1DI.xlsx
+++ b/form_reporting_templates/Form-1DI.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\iotc-reference-forms\form_reporting_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\repositories\data_dissemination\iotc-reference-forms\form_reporting_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4792399-A0F1-4C93-8701-8A4969D7A8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EAE40F-45CD-40D1-97BD-9F3A5D5F5977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Z3raniWjLRXszYCbzXa/TU1R8wd1kHrHNccmNn7mHkAZRDJmvrP7BMraCIbrDBSr6tBMzuhQ6TxYUg6cyC/1Bg==" workbookSaltValue="C01nC0I7gdRYfsDcA3RybQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -1073,58 +1073,58 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1473,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,7 +1756,7 @@
       <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7U7/Qt/9oOtBEff6qv3dYDnEa1ebiJlsXJoJOPJWthLKwyFXhTQmUxAB8ybSQNAAbfVsXr3lqKewQd/wnoKImg==" saltValue="2Pzu5Tizz9+r1G0lldUyRg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Y/eggeJdu3lbDMBAFFlxYkSjmDZsPe2+GxkxhetXgxXb/7qL09G7nEtPR8dyNLXA1mazUzwGIwTYtSWVkl7z6w==" saltValue="wMiGgKYF8B6I1klAW3sOxg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="4">
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C8:D8"/>
@@ -1770,7 +1770,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C19" r:id="rId1" location="entities" xr:uid="{3E135360-8976-4AAA-8474-BB32F06C9745}"/>
-    <hyperlink ref="C20" r:id="rId2" location="countries" display="Flag country" xr:uid="{F730E8AF-D3A7-4431-9DD3-422CC542A285}"/>
+    <hyperlink ref="C20" r:id="rId2" location="countries" xr:uid="{F730E8AF-D3A7-4431-9DD3-422CC542A285}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1781,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:HC1048575"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="11" ySplit="7" topLeftCell="L8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -4073,7 +4073,7 @@
       <c r="HC1048575" s="46"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7y30xUDt19rWnUkEQecomBB6U3TesPo1zIQt5KuetdcxPNveuCy0au6mtZqQUzv9gQBEfL6GPDrN1yO8U17XeA==" saltValue="PQ1Y3bVNWcuOHWop+u1utg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="9RkriDZ24gD60wzrGIfYg0lQq3InhGzoxnCGxNes2nFcjEMORq/xdopyRw1rU1tuYB0mT1OW4T29ks9PWzzScQ==" saltValue="q4Y66gLudP/Se8ARWgDJhw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="B4:E6"/>
     <mergeCell ref="F4:H6"/>
@@ -4103,9 +4103,9 @@
     <hyperlink ref="G7" r:id="rId3" location="sourcesDI" xr:uid="{87C22EDC-E88B-47B5-A906-5136A2DCB1A3}"/>
     <hyperlink ref="H7" r:id="rId4" location="processingsDI" xr:uid="{5D715338-F6EA-4526-A9D0-7C9B67DA75F5}"/>
     <hyperlink ref="I7" r:id="rId5" location="coverageTypes" xr:uid="{FCADF32B-4240-49F8-9CD4-8D05AA29176A}"/>
-    <hyperlink ref="K7" r:id="rId6" location="catchUnits" display="Discard unit" xr:uid="{8E2457EF-BFD9-4480-93F6-844FC19CD52F}"/>
+    <hyperlink ref="K7" r:id="rId6" location="catchUnits" xr:uid="{8E2457EF-BFD9-4480-93F6-844FC19CD52F}"/>
     <hyperlink ref="C7" r:id="rId7" location="fisheries" xr:uid="{F95149BA-1BB2-46CC-A86F-36B6AC4AFBA6}"/>
-    <hyperlink ref="E7" r:id="rId8" location="discardReasons" display="Disc. reason" xr:uid="{4B127CA8-AB4F-43B9-B5B8-5A77A85A9028}"/>
+    <hyperlink ref="E7" r:id="rId8" location="discardReasons" xr:uid="{4B127CA8-AB4F-43B9-B5B8-5A77A85A9028}"/>
     <hyperlink ref="K4" r:id="rId9" location="species" xr:uid="{0BBE03AC-0AAA-41DA-99E5-9DD325DC155B}"/>
     <hyperlink ref="K5" r:id="rId10" location="individualConditions" xr:uid="{431CFE87-EEB6-4BEC-9E8B-1A482800044E}"/>
     <hyperlink ref="K6" r:id="rId11" location="raisings" xr:uid="{387C7B1D-B99F-4149-9A85-EE0666628CB0}"/>

</xml_diff>